<commit_message>
1 file upload and QA update
</commit_message>
<xml_diff>
--- a/QA.xlsx
+++ b/QA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="296">
   <si>
     <t>Q</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -285,10 +285,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>노인장기요양보험,장기요양급여</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>장기요양급여,종류</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -561,6 +557,533 @@
   </si>
   <si>
     <t>대한노인회 노인자원봉사지원센터지역운영본부</t>
+  </si>
+  <si>
+    <t>치매</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개념</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>치매란 뭐야?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>퇴행성 뇌질환 또는 뇌혈관계 질환 등으로 인해 기억력, 언어능력, 지남력(指南力), 판단력 및 수행능력 등의 기능이 저하됨으로써 일상생활에서 지장을 초래하는 후천적인 다발성 장애</t>
+  </si>
+  <si>
+    <t>paragraph</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>단계</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대화 중 그것, 저것으로 표현하시는 데 어떤 치매 단계이니?</t>
+  </si>
+  <si>
+    <t>초기 치매</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>치매란 퇴행성 뇌질환 또는 뇌혈관계 질환 등으로 인해 기억력, 언어능력, 지남력(指南力), 판단력 및 수행능력 등의 기능이 저하됨으로써 일상생활에서 지장을 초래하는 후천적인 다발성 장애를 말합니다. 치매의 증상은 인지 증상과 정신행동 증상으로 나눌 수 있습니다. 인지 증상이란 기억력, 언어 기능, 시간 지남력, 시공간능력 그리고 수행능력의 저하되는 증상입니다. 예를 들어, 최근의 말이나 사건에 대해서 기억을 하지 못하거나 사물이나 사람의 이름이 기억이 나지 않으면 치매 증상이 나타나는 것입니다. 또한 날짜와 시간에 대한 감각이 없고 자주 다니던 길을 잃고 헤매거나 집안의 간단한 도구를 다루지 못하는 경우도 치매 증상이 나타나는 경우입니다. 정신행동 증상이란 급격한 성격 변화가 있거나 우울하고 초조한 기분이 들고 환각이나 망상을 하는 증상입니다. 예를 들어, 예전의 성격이 강해지거나 충동의 조절이 안 되고 슬프거나 기분이 쳐진 것처럼 행동하는 경우는 치매 증상이 나타나는 경우입니다. 그리고 가만히 있지를 못하고 목적 없이 자꾸 움직이며 실제로는 없는 소리나 사물, 사람을 보거나 듣거나 자신의 돈이나 사물을 다른 사람이 훔쳐 갔다고 주장하는 경우도 치매 증상이 나타나는 경우입니다. 마지막으로 주변에 대한 관심과 흥미를 잃고 새로운 일을 시작하려는 의욕이 감소하는 경우도 치매 증상 중 하나입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>의사가 저희 아버지께서 치매의 중기에 있다고 합니다. 무슨 의미인가요?</t>
+  </si>
+  <si>
+    <t>기본적으로 생활하는 데 도움이 필요한 상태</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 치매는 그 진행과정에 따라 초기,중기,말기로 구분할 수 있습니다. 진행성 질환인 치매는 시간의 흐름에 따라 증상의 양상과 심각도가 변하므로, 병의 양상을 이해하고 어떻게 케어할 것인가를 결정하는 기준이 필요합니다. 대략적으로 초기는 기본적인 생활능력이 유지되는 상태이고, 중기는 기본적으로 생활하는 데 도움이 필요한 상태입니다. 말기에는 기본적인 생활을 타인에게 전적으로 의존해야 하는 상태입니다. 초기는 가족이나 동료들이 문제가 있음을 알아차리기 시작하나, 아직은 혼자서 지낼 수 있는 수준입니다. 예전 기억은 유지되나 최근에 있었던 일을 잊어버리거나 음식을 조리하다가 불 끄는 것을 자주 잊어버리는 경우 초기 치매입니다. 또한 미리 적어 두지 않으면 중요한 약속을 잊어버리거나 조금 전에 했던 말을 반복하거나 질문을 되풀이하는 경우 초기 치매입니다. 마지막으로 대화 중 정확한 단어가 떠오르지 않아 ‘그것’, ‘저것’으로 표현하거나 머뭇거릴 때 초기 치매입니다. 
+ 중기는 치매임을 쉽게 알 수 있는 단계로 어느 정도의 도움 없이는 혼자 지낼 수 없는 수준입니다. 돈 계산이 서툴러지고 전화, TV 등 가전제품을 조작하지 못하는 경우 중기 치매입니다. 또한 중기 치매일 경우에 며칠인지, 몇 시인지, 어느 계절인지, 자신이 어디에 있는지 등을 파악하지 못하며 평소 잘 알고 지내던 사람을 혼동하기시작하지만 대부분 가족은 알아봅니다. 그리고 익숙한 장소임에도 불구하고 길을 자주 잃어버리는 경우도 중기 치매입니다. 
+ 말기는 인지기능이 현저히 저하되고 정신행동 증상과 아울러 신경학적 증상 및 기타 신체적합병증 등이 동반되어 독립적인 생활이 거의 불가능한 수준입니다. 말기 치매일 경우에 식사, 옷 입기, 세수하기, 대소변 가리기 등 완전히 다른 사람의 도움을 필요로 합니다. 말기 치매일 때 대부분의 기억이 상실되며 배우자나 자식을 알아보지 못합니다. 또한 말기 치매이면 혼자 웅얼거리거나 전혀 말을 하지 못하며 의미 있는 판단을 내릴 수 없고, 간단한 지시도 따르지 못합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>진단</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>치매 진단을 내릴 때 어떤 검사를 받게 되나요?</t>
+  </si>
+  <si>
+    <t>병력 조사, 의사의 진찰, 검사실 검사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 치매는 매우 다양한 원인에 의해 생기기 때문에 한 가지 검사로 진단을 내릴 수 없습니다. 따라서 전문의에게 의뢰하게 되면 병력 조사, 의사의 진찰, 검사실 검사를 받게 되며 이를 통해 진단을 내리게 됩니다. 첫째, 자세한 병력 조사입니다. 병력조사란 언제부터 증세가 시작되었고, 어떤 증세가 주로 나타났으며, 지금까지 어떤 변화를 겪어왔는지를 자세히 알아보는 과정을 말합니다. 첨단 기계를 사용하는 검사과정보다 이러한 문진 과정이 훨씬 더 중요합니다. 일단 증상에 대한 전반적인 파악이 되면 치매의 원인이 될 수 있는 질환이 혹시 있는지의 여부도 묻게 됩니다. 고혈압, 당뇨, 고지혈증, 체중의 급격한 변화, 과거의 신체 질환들, 뇌 손상 여부, 알코올이나 다른 약물에 대한 중독 여부 등이 정확한 진단에 중요한 단서를 제공할 수 있습니다.
+ 둘째, 직접 진찰하는 과정입니다. 이 과정은 신체검사, 신경학적 검사, 정신상태 검사 등 세 가지로 이루어지는데, 혈압, 체온, 맥박 등의 측정과 전신의 각 부분에 대한 진찰을 하고, 이어서 감각, 운동 신경이나 근육의 위축, 보행능력, 반사운동 등 각종 신경학적 기능도 평가하게 됩니다. 정신상태 검사는 우울증과 불안, 공포증, 망상 등의 정신현상을 평가하는 과정을 말합니다.
+ 셋째, 검사실 검사 과정입니다. 위의 두 과정을 거친 후, 대부분의 경험 많은 치매 전문가들은 환자가 치매를 앓고 있는지의 여부, 또 치매가 있다면 어떤 종류의 치매인지를 개략적으로 추정할 수 있지만, 확진을 위해서는 각종 검사 과정이
+필요합니다. 검사 과정은 신체질환의 여부를 확인하기 위한 검사실 검사, 뇌 기능을 평가하기 위한 신경인지기능 검사 및 뇌의 구조와 기능을 보기 위한 뇌영상 검사로 구분됩니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예방</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>치매예방수칙이 뭐야?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>치매예방수칙 333은 3권(勸, 즐길 것), 3금(禁, 참을 것), 3행(行, 챙길 것)</t>
+  </si>
+  <si>
+    <t>치매예방수칙에서 3권이 뭐니?</t>
+  </si>
+  <si>
+    <t>일주일에 3번 이상 걷기, 식사를 거르지 말고 생선과 채소를 골고루 챙기기 그리고 틈날 때마다 독서하기</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 치매의 정확한 원인은 밝혀지지 않았지만 노화와 치매를 예방하기 위해 뇌의 염증, 영양 부족, 수면 부족, 알코올 등의 독소, 당뇨 등이 중요한 원인이 될 수 있으니 생활습관에 유의해야 합니다. 치매의 경우 예방 접종과 같은 확실한 예방법이 있는 것은 아니지만, 치매의 발병 위험성을 높일 수 있는 인자들을 미리 조절함으로써 치매에 걸릴 확률을 줄일 수 있습니다. 뇌세포는 일단 손상되면 재생되지 않기 때문에 치매에 대한 예방이 매우 중요합니다. 치매는 건강한 생활을 통해서 상당 부분이 예방이 가능하며, 치매예방수칙 333을 잘 인식하고 실천해야 합니다. 치매예방수칙 333은 3권(勸, 즐길 것), 3금(禁, 참을 것), 3행(行, 챙길 것)을 뜻합니다. 치매예방수칙 333의 첫번째 수칙인 3권(勸, 즐길 것)은 일주일에 3번 이상 걷기, 식사를 거르지 말고 생선과 채소를 골고루 챙기기 그리고 틈날 때마다 독서하기입니다. 두번째 수칙인 3금(禁, 참을 것)은 술은 한 번에 3잔보다 적게 마시기, 담배는 피우지 말기(금연) 그리고 머리를 다치지 않도록 조심하기입니다. 세번째 수칙인 3행(行, 챙길 것)은 혈압,혈당,콜레스트롤 3가지를 정기적으로 체크하기, 가족과 친구에게 자주 연락하고 만나기 그리고 매년 보건소에서 치매 조기검진 받기입니다. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 치매의 정확한 원인은 밝혀지지 않았지만 노화와 치매를 예방하기 위해 뇌의 염증, 영양 부족, 수면 부족, 알코올 등의 독소, 당뇨 등이 중요한 원인이 될 수 있으니 생활습관에 유의해야 합니다. 치매의 경우 예방 접종과 같은 확실한 예방법이 있는 것은 아니지만, 치매의 발병 위험성을 높일 수 있는 인자들을 미리 조절함으로써 치매에 걸릴 확률을 줄일 수 있습니다. 뇌세포는 일단 손상되면 재생되지 않기 때문에 치매에 대한 예방이 매우 중요합니다. 치매는 건강한 생활을 통해서 상당 부분이 예방이 가능하며, 치매예방수칙 333을 잘 인식하고 실천해야 합니다. 치매예방수칙 333은 3권(勸, 즐길 것), 3금(禁, 참을 것), 3행(行, 챙길 것)을 뜻합니다. 치매예방수칙 333의 첫번째 수칙인 3권(勸, 즐길 것)은 일주일에 3번 이상 걷기, 식사를 거르지 말고 생선과 채소를 골고루 챙기기 그리고 틈날 때마다 독서하기입니다. 두번째 수칙인 3금(禁, 참을 것)은 술은 한 번에 3잔보다 적게 마시기, 담배는 피우지 말기(금연) 그리고 머리를 다치지 않도록 조심하기입니다. 세번째 수칙인 3행(行, 챙길 것)은 혈압,혈당,콜레스트롤 4가지를 정기적으로 체크하기, 가족과 친구에게 자주 연락하고 만나기 그리고 매년 보건소에서 치매 조기검진 받기입니다.</t>
+  </si>
+  <si>
+    <t>치매검진사업에서는 무슨 서비스를 제공하니?</t>
+  </si>
+  <si>
+    <t>치매검진사업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>만 60세 이상의 어르신께 무료검진</t>
+  </si>
+  <si>
+    <t>치매검진사업에서 선별검사 대상자인데 보건소를 못 갈 것 같아. 혹시 다른 방안이 있니?</t>
+  </si>
+  <si>
+    <t>찾아가는 치매검사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">치매는 다양한 원인에 의해 발생되며 조기에 발견하여 적절히 치료할 경우 완치 또는 중증 상태로의 진행을 억제시키거나 증상을 개선하는 것이 가능합니다. 치매검진사업은 치매 환자와 그 가족의 고통과 부담을 크게 경감시키고 치매로 인한 사회적 비용도 절감하기 위하여 보건복지부에서 실시되는 사업으로 만 60세 이상의 어르신께 무료검진을 제공합니다. 치매검진사업에서는 치매 가능성이 높은 대상자를 가려내기 위한 선별검사와 치매진단을 위한 정밀검사로 구분되어 검진을 실시합니다. 치매안심센터 주소지 관할 거주 만 60세 이상으로 치매로 진단받지 않은 모든 주민은 선별검사 대상자입니다. 선별검사 대상자는 주소지 관할 치매안심센터에서 간이정신 상태검사(MMSE-DS)를 통해 인지감퇴가 있는지를 평가받게 됩니다. 다만, 대상자가 골절 및 중증질환 등 불가피한 경우 방문 검진을 시행하며, 방문 검시 시 주변의 방해를 받지 않고 검진을 시행할 수 있는 독립된 공간 확보돼야 합니다.  선별 검사에서 보건소 '찾아가는 치매검사' 실시합니다. 도서벽지 등 취약지역에 보건소 방문이 어려운 독거노인, 취약계층 노인, 치매 고위험군 노인 등을 대상으로 경로당, 노인복지관, 노인회관, 보건예방교육 등을 통한 찾아가는 치매 검사로 조기 검진을 확대 실시합니다. 
+ 선별검사 결과 ‘인지저하’로 판정된 자, ‘정상’이나 치매 의심증상(인지저하 의심군)이 뚜렷하여 진단검사가 필요하다고 판단되는 자는 협력의사와 면담(진료)을 한 후 치매안심센터 임상심리사 또는 시행훈련을 받은 간호사에게 신경심리검사와 협력병원 의사를 통하여 치매 임상 평가를 받게 됩니다. 이에 따라 치매, 경도인지장애, 정상 여부를 진단합니다. 마지막으로 치매 진단검사 결과 치매의 원인에 대한 감별검사가 필요한 자는 협약병원에서 혈액검사와 소변검사 및 뇌영상검사(CT)를 통해 치매의 원인질환이 무엇인지를 평가받게 됩니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>치매는 다양한 원인에 의해 발생되며 조기에 발견하여 적절히 치료할 경우 완치 또는 중증 상태로의 진행을 억제시키거나 증상을 개선하는 것이 가능합니다. 치매검진사업은 치매 환자와 그 가족의 고통과 부담을 크게 경감시키고 치매로 인한 사회적 비용도 절감하기 위하여 보건복지부에서 실시되는 사업으로 만 60세 이상의 어르신께 무료검진을 제공합니다. 치매검진사업에서는 치매 가능성이 높은 대상자를 가려내기 위한 선별검사와 치매진단을 위한 정밀검사로 구분되어 검진을 실시합니다. 치매안심센터 주소지 관할 거주 만 61세 이상으로 치매로 진단받지 않은 모든 주민은 선별검사 대상자입니다. 선별검사 대상자는 주소지 관할 치매안심센터에서 간이정신 상태검사(MMSE-DS)를 통해 인지감퇴가 있는지를 평가받게 됩니다. 다만, 대상자가 골절 및 중증질환 등 불가피한 경우 방문 검진을 시행하며, 방문 검시 시 주변의 방해를 받지 않고 검진을 시행할 수 있는 독립된 공간 확보돼야 합니다.  선별 검사에서 보건소 '찾아가는 치매검사' 실시합니다. 도서벽지 등 취약지역에 보건소 방문이 어려운 독거노인, 취약계층 노인, 치매 고위험군 노인 등을 대상으로 경로당, 노인복지관, 노인회관, 보건예방교육 등을 통한 찾아가는 치매 검사로 조기 검진을 확대 실시합니다. 
+ 선별검사 결과 ‘인지저하’로 판정된 자, ‘정상’이나 치매 의심증상(인지저하 의심군)이 뚜렷하여 진단검사가 필요하다고 판단되는 자는 협력의사와 면담(진료)을 한 후 치매안심센터 임상심리사 또는 시행훈련을 받은 간호사에게 신경심리검사와 협력병원 의사를 통하여 치매 임상 평가를 받게 됩니다. 이에 따라 치매, 경도인지장애, 정상 여부를 진단합니다. 마지막으로 치매 진단검사 결과 치매의 원인에 대한 감별검사가 필요한 자는 협약병원에서 혈액검사와 소변검사 및 뇌영상검사(CT)를 통해 치매의 원인질환이 무엇인지를 평가받게 됩니다.</t>
+  </si>
+  <si>
+    <t>치매를 진단받아서 MRI 검사를 받았는데 얼마 정도 비용을 지원받니?</t>
+  </si>
+  <si>
+    <t>치매검진,비용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1인당 상한 8만원~11만원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 치매검진을 받는 사람 중 만 60세 이상의 의료급여 수급자, 국민건강보험 가입자 및 피부양자 중에서 소득과 재산 등을 기준으로 치매검진 비용을 지원합니다. 검진비용 대상자는 기준 중위소득 120% 이하여야 합니다. 전문의 진찰, 치매척도검사, 치매신경인지검사 등인 진담 검사를 받았을 경우에 1인당 상한 15만원 정도의 치매검진 비용을 지원합니다. 또한 혈액성분검사, 전해질 검사, 신장기능검사, 간기능검사, 갑상선기능검사, 혈당검사, 요산검사, 콜레스테롤 검사, 매독검사, 요검사, 뇌영상촬영(CT 또는 MRI)인 감별 검사를 받았을 경우에 1인당 상한 8만원~11만원 정도의 치매검진 비용을 지원합니다. </t>
+  </si>
+  <si>
+    <t>국민건강보험공단에서 실시하는 치매선별검사를 받고 싶어. 어디로 가야하니?</t>
+  </si>
+  <si>
+    <t>국민건강보험공단</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>국민건강보험공단에서 지정한 건강검진기관</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 국민건강보험공단에서 66세, 70세, 74세 노인에게 치매선별검사 및 인지기능장애 검사를 제공하고, 지역사회 보건소와 연계한 상담서비스를 제공합니다. 국민건강보험공단에서 1차 검진 시에 치매선별검사를 실시하고, 1차 수검자 중 인지기능장애 고위험군 노인을 대상으로 인지기능장애 검사 및 상담 서비스를 제공합니다. 66세 노인은 “생애전환기 건강진단”을 통해, 70세 및 74세 노인은 2년 주기의 “일반건강검진”을 통해 치매조기검진서비스를 제공합니다. 국민건강보험공단에서 지정한 건강검진기관에서 검진을 받을 수 있습니다. </t>
+  </si>
+  <si>
+    <t>관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 치매 조기검진을 통해 치매, 치매고위험군, 정상 중 한 가지로 판정을 받거나 전문의료기관에서 이미 치매로 진단을 받은 대상자는 보건소에 설치된 치매상담센터에 등록되어 각 구분에 따라 정상 관리 서비스, 치매위험군 관리 서비스, 치매 관리 서비스를 제공받습니다. 정상 관리 서비스는 정기선별검진 서비스, 치매예방 정보제공 서비스, 치매예방 관련 프로그램 연계 서비스, 기타 필요한 서비스입니다. 치매위험군 관리 서비스는 정기 정밀검진 서비스, 인지건강센터 프로그램 시행, 치매예방 정보제공 서비스, 치매예방 관련 프로그램 연계 서비스 그리고 기타 필요한 서비스입니다. 치매 관리 서비스는 인지건강센터 프로그램 시행, 방문간호 서비스, 조호물품 제공 서비스(위생재료 무상공급, 조호기구 무상대여), 배회가능어르신(배회인식표, 팔찌, GPS 보급 및사전 지문등록 연계 실시), 치매관련 정보 제공, 가족모임(또는 가족교실), 지역 치매관련 자원연계(의료기관, 복지시설 등 연계), 치료비 지원(저소득층) 등입니다. 
+ 치매예방 및 치매환자 관리 등에 관한 전문적이고 체계적인 상담 서비스를 제공하기 위해 보건소에서 치매안심센터와 치매상담전화센터를 운영하고 있습니다. 치매안심센터는 치매관련 상담 및 조기검진, 환자의 등록·관리, 치매등록통계사업의 지원과 같은 업무를 담당하고 있습니다. 치매상담전화센터는 치매에 관한 정보를 제공할 뿐만 아니라 치매환자와 그 가족의 치료·보호 및 관리에 관한 정보를 제공합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정상 관리 서비스, 치매위험군 관리 서비스, 치매 관리 서비스</t>
+  </si>
+  <si>
+    <t>할머니가 치매환자이신데 보건소의 치매 센터에 등록하며 무슨 서비스를 받니?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>치매환자가 연간 얼마나 의료비를 지원받을 수 있나요?</t>
+  </si>
+  <si>
+    <t>36만원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">치매 환자가 있는 4인 가구 소득이 얼마여야 치료비를 지원받을 수 있나요? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,699,000원 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 국가와 지방자치단체는 치매환자의 경제적 부담능력을 고려하여 치매 치료 및 진단에 드는 비용을 지원할 수 있습니다. 건강보험가입자 및 피부양자 중 치매환자, 의료급여수급권자 중 치매환자 중에서 소득과 재산 등이 기준 중위소득 120% 이하인 사람은 의료비를 지원받을 수 있습니다. 2020년 가구 규모별 소득기준은 1인 가구일 경우에 2,109,000원, 2인 가구일 경우에 3,590,000원, 3인 가구일 경우에 4,645,000원, 4인 가구일 경우에 5,699,000원 5인 가구일 경우에 6,753,000원이며, 가구당 해당 소득의 이하일 경우에 치료비를 지원받을 수 있습니다. 2020년 1월 1일부터 12월 31일까지 치매치료관리비 보험급여분 중 중 본인부담금에 대해 치료비를 월 3만원(연간 36만원) 한도 내에서 지원받습니다. 
+ 치료비를 지원받으려는 사람은 관할 보건소장에게 지원신청서, 대상자 본인 명의 입금 통장 사본 1부, 당해 연도에 발행된 치매치료제가 포함된 약처방전 또는 약품명이 기재된 약국 영수증을 제출해야 합니다. 치료비 지원 신청을 받은 보건소장은 관계 기관에 의료비 지원 대상자의 소득·재산 등에 관한 자료제출을 요청할 수 있습니다. 보건소(치매안심센터)에 치매환자로 등록된 자 중에서 지원대상자 선정기준(① 연령기준, ② 진단기준, ③치료기준, ④소득기준)에 적합한 자를 지원 대상자로 선정합니다. 다만, 신청자 중에서 보훈대상자 의료지원 등 중복 지원은 되지 않습니다. 신청자 중에서 대상자 선정기준에 적합한 사람이 지원대상자로 선정되면 신청일로부터 14일 이내에 그 결과를 통지받습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 국가와 지방자치단체는 치매환자의 경제적 부담능력을 고려하여 치매 치료 및 진단에 드는 비용을 지원할 수 있습니다. 건강보험가입자 및 피부양자 중 치매환자, 의료급여수급권자 중 치매환자 중에서 소득과 재산 등이 기준 중위소득 120% 이하인 사람은 의료비를 지원받을 수 있습니다. 2020년 가구 규모별 소득기준은 1인 가구일 경우에 2,109,000원, 2인 가구일 경우에 3,590,000원, 3인 가구일 경우에 4,645,000원, 4인 가구일 경우에 5,699,000원 5인 가구일 경우에 6,753,000원이며, 가구당 해당 소득의 이하일 경우에 치료비를 지원받을 수 있습니다. 2020년 1월 1일부터 12월 31일까지 치매치료관리비 보험급여분 중 중 본인부담금에 대해 치료비를 월 3만원(연간 36만원) 한도 내에서 지원받습니다. 
+ 치료비를 지원받으려는 사람은 관할 보건소장에게 지원신청서, 대상자 본인 명의 입금 통장 사본 1부, 당해 연도에 발행된 치매치료제가 포함된 약처방전 또는 약품명이 기재된 약국 영수증을 제출해야 합니다. 치료비 지원 신청을 받은 보건소장은 관계 기관에 의료비 지원 대상자의 소득·재산 등에 관한 자료제출을 요청할 수 있습니다. 보건소(치매안심센터)에 치매환자로 등록된 자 중에서 지원대상자 선정기준(① 연령기준, ② 진단기준, ③치료기준, ④소득기준)에 적합한 자를 지원 대상자로 선정합니다. 다만, 신청자 중에서 보훈대상자 의료지원 등 중복 지원은 되지 않습니다. 신청자 중에서 대상자 선정기준에 적합한 사람이 지원대상자로 선정되면 신청일로부터 13일 이내에 그 결과를 통지받습니다.</t>
+  </si>
+  <si>
+    <t>할머니께서 치매 환자이신데 한 달 동안 저희 가족이 돌봐드리지 못할 것 같습니다. 혹시 추천해줄만한 치매 시설이 있나요?</t>
+  </si>
+  <si>
+    <t>주야간 보호시설, 단기보호시설, 노인요양시설, 노인요양 공동생활가정, 요양병원</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 치매 관련 시설에는 주야간 보호시설, 단기보호시설, 노인요양시설, 노인요양 공동생활가정, 요양병원이 있습니다. 주야간 보호시설은 일정기간 동안 보살핌이 필요하며 심신기능 유지 및 향상이 필요한 어르신에게 적합합니다. 단기보호시설은 부득이한 사정에 의해 일시적으로 보호가 필요한 어르신에게 적합합니다. 노인요양시설은 안정적인 상태를 유지하고 있는 어르신에게 적합합니다. 노인요양 공동생활가정은 심신에 장애가 발생하여 가정과 같은 주거 여건과 급식, 요양 및 일상 생활에 편의를 필요로 하는 어르신에게 적합합니다. 요양병원은 지속적으로 의료적 처치와 관찰이 필요한 어르신에게 적합합니다. 
+ 치매 노인을 위한 여러 시설들은 이름도 다양하며 기능도 약간씩 차이가 있습니다. 시설이라고 모두가 치매 노인에게 적당한 것은 아니며, 병의 경과에 따라 적절한 시설이 달라질 수 있습니다. 치매 노인의 상태에 따라 거동이 가능한 경증 노인은 주야간 보호 등 재가서비스를 이용하고, 이보다 상태가 심각한 경우에는 요양원 입소를 고려할 수 있으며, 질환으로 인한 치료나 수술 후 재활 등이 필요한 경우에는 요양병원을 이용할 수 있습니다. 치매 노인의 경우 신체 상태의 악화보다는 돌봄 요구도의 증가가 입소 결정을 내리는데 중요한 이유가 됩니다. 문제행동, 돌봄자의 건강 악화 및 부담 증가, 인지기능 감퇴 등의 문제들이 더해져서 환자를 요양시설로 입소시키는 결정이 내려지게 됩니다. 
+ 치매 노인의 생활 안정과 심신기능의 유지 및 향상이 필요할 때이거나 부득이한 사유로 가족의 보호를 받을 수 없어 일시적으로 보호가 필요할 때 시설에 입소를 고려해야 합니다. 또한, 가족이 더 이상 환자의 일상생활을 도와 줄 수 없을 때, 치매 노인의 망상과 환각 등 심각한 정신행동 증상으로 타인과 공동생활이 어려울 때, 치매에 병발된 신체 질환으로 인해 지속적 치료가 필요할 때에 시설 입소를 고려해야 합니다. 시설에 입소하는 경우 비용, 위치, 프로그램, 안전대책 등을 고려하여 시설을 선택해야 합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>할머니가 치매 환자이신데 시설급여는 얼마나 지원받니?</t>
+  </si>
+  <si>
+    <t>시설,선택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시설,입소비용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>치매로 인해 요양을 필요로 하는 65세 이상의 노인은 노인의료복지시설에 입소하여 급식·요양 그 밖의 일상생활에 필요한 편의를 제공받을 수 있도록 시설급여를 제공합니다. “시설급여”란 장기요양기관에 장기간 입소한 수급자에게 신체활동 지원 및 심신기능의 유지·향상을 위한 교육·훈련 등을 제공하는 장기요양급여를 말합니다. 시설급여를 제공할 수 있는 장기요양기관은 노인요양시설과 노인요양공동생활가정이 있습니다. 시설급여 비용은 일반대상자의 경우 총 급여비용 중 20%를 수급자 본인이 부담하고, 80%는 공단에서 장기요양기관에 지급합니다. 의료급여 수급권자, 고시하는 지역에 거주하고 피해정도가 일정 기준에 이르는 생계곤란자는 본인부담금의 60%의 범위에서 보건복지부장관이 정하는 바에 따라 차등하여 감경할 수 있습니다. 식사재료비, 이·미용비, 대상자의 요청에 의한 상급침실(1-2인실) 이용에 따른 추가비용은 시설급여 비용에서 제외되므로 전액 본인이 추가로 부담해야 합니다. 장기요양등급 4등급 및 5등급 수급자가 시설급여를 이용하는 경우 3등급 급여비용이 산정됩니다. 또한 장기요양급여의 월 한도액을 초과하는 비용은 수급자 본인이 전부 부담해야 합니다. 생계급여 수급자, 의료급여 수급자 및 부양의무자로부터 적절한 부양을 받지 못하는 65세 이상의 사람은 국가 및 지방자치단체가 전액 부담합니다. 입소자로부터 입소비용의 전부를 수납하여 운영하는 노인요양시설 또는 노인요양공동생활가정 입소대상자는 입소자 본인이 전액 부담합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반대상자의 경우 총 급여비용 중 20%를 수급자 본인이 부담하고, 80%는 공단에서 장기요양기관에 지급</t>
+  </si>
+  <si>
+    <t>치매 환자를 위한 가정 방문 서비스가 있니?</t>
+  </si>
+  <si>
+    <t>가정 방문요양 서비스</t>
+  </si>
+  <si>
+    <t>가정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>치매 노인이 있는 가족은 가족요양비를 지급받을 수 있다고 들었어. 얼마 정도 지급받니?</t>
+  </si>
+  <si>
+    <t>가족요양비</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>월 150,000원</t>
+  </si>
+  <si>
+    <t xml:space="preserve">국민건강보험공단은 치매 노인의 가족 등으로부터 방문요양에 상당한 장기요양급여를 받은 경우 해당 수급자에게 가족요양비를 지급할 수 있습니다. 다만, 이때 가족요양비를 지급받는 조건은 치매 노인이 섬·벽지 등 장기요양기관이 현저히 부족한 지역에 거주하는 사람, 천재지변이나 그 밖에 이와 유사한 사유로 인하여 장기요양기관이 제공하는 장기요양급여를 이용하기가 어렵다고 보건복지부장관이 인정하는 사람, 감염병환자, 정신장애인 중 하나여야 합니다. 가족요양비는 장기요양등급에 관계없이 월 150,000원을 지급합니다. 가족요양비를 지급받으려는 사람은 가족요양비 지급신청서를 공단이 등급판정위원회에 자료를 제출하기 전까지 공단에 제출해야 합니다. 만약 감염병환자로서 감염의 위험성이 있는 사람이 가족요양비를 신청할 때에는 진단서를 공단에 제출해야 합니다. 또한 정신장애인이 가족요양비를 신청할 경우에 장애인등록증을 제출해야 합니다. 신체적 변형 등의 사유로 대인과의 접촉을 기피하는 자가 가족요양비를 신청할 경우, 진단서 등 이를 증명할 수 있는 서류를 제출해야 합니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">치매로 인해 독립적인 일상생활을 수행하기 곤란한 노인과 치매 노인 부양가정에 필요한 각종 서비스를 제공함으로써, 치매 노인이 가족 및 친지와 더불어 건강하고 안정된 노후 생활을 영위할 수 있도록 함과 동시에 치매 노인부양으로 인한 가족의 부담을 덜어주기 위해 재가급여를 제공합니다. 가정에서 일상생활을 영위하고 있는 노인으로서 치매로 인하여 신체적·정신적 장애로 어려움을 겪고 있는 노인에게 지역사회 안에서 건전하고 안정된 노후를 영위하도록 장기요양요원이 가정을 방문하여 신체활동 및 가사활동 등 필요한 각종 서비스를 제공합니다. 가정 방문요양 서비스는 장기요양급여수급자(1-5등급)이거나 심신이 허약하거나 장애가 있는 65세 이상의 사람으로서 가정에서의 보호가 필요한 사람이 이용할 수 있습니다. 장기요양요원이 치매환자를 위해 가정을 방문하여 말벗이 되어주며 세면도움, 구강관리, 몸 청결 등의 신체활동을 지원하고 취사, 생활필수품 구매를 대신 수행합니다. 자세한 내용은 재가노인복지시설에 대한 생활법령을 참고하면 됩니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>치매 환자가 있는 가족을 지원하는 사업이 있니? 자세히 알려줘</t>
+  </si>
+  <si>
+    <t>치매가족 및 보호자 지원사업</t>
+  </si>
+  <si>
+    <t>치매 지원사업에서 돌봄에 대한 스트레스를 완화시켜주는 프로그램이 있니?</t>
+  </si>
+  <si>
+    <t>힐링 프로그램</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>“치매가족 및 보호자 지원사업”이란 치매환자 가족 및 보호자에게 환자돌봄에 대한 지원을 통하여 치매에 대한 이해를 높이고 환자의 돌봄 부담을 경감하기 위한 사업입니다. 치매환자가족 및 보호자 상담 및 돌봄부담 분석, 가족교실 운영, 자조모임 지원, 힐링 프로그램, 치매가족 카페 운영, 동반치매환자보호서비스를 지원합니다. 이 사업에서 관할 치매안심센터 방문 또는 전화 예약을 통해 치매환자가족 및 보호자 상담을 통해 돌봄부담 요인을 파악하고 부담 경감에 필요한 적절한 서비스를 연계해드립니다. 또한 치매가족 및 보호자 지원사업은 가족 교실의 체계적이고 구체적인 커리큘럼을 통해 치매환자 가족의 치매 및 환자돌봄에 대한 이해와 돌봄역량을 향상시켜 드립니다. 사업에서 치매환자 가족 간 정서 및 정보 교류를 통해 심리적 부담 경감과 사회적 고립을 방지할 수 있도록 정기적 모임을 지원해 드립니다. 그리고 치매환자와 가족이 함께 참여할 수 있는 다양한 힐링 프로그램을 통해, 상호 간 스트레스를 해소하고 정서적 교류와 심리적 부담을 경감하도록 지원해 드립니다. 치매환자와 가족이 편안하게 방문하여, 함께 휴식을 취하고 다른 치매환자 및 가족과 교류할 수 있는 장소를 제공해 드립니다. 치매관련 정보 제공을 통해 치매에 관심이 있는 지역주민의 치매에 대한 인식 개선 및 올바른 지식 함양을 도모할 수 있도록 지원해 드립니다. 치매환자가족이 안심센터 가족프로그램을 참여하는 동안 동반한 치매환자를 보호하여 가족의 프로그램 참여를 독려하고 지원해 드립니다. 가족교실, 자조모임, 힐링프로그램 등 치매안심센터 내부에서 진행되는 가족 프로그램에 참여하는 경우에 이용할 수 있습니다.</t>
+  </si>
+  <si>
+    <t>사전등록제를 통해 치매 노인을 전보다 더 빨리 찾을 수 있나요?</t>
+  </si>
+  <si>
+    <t>사전등록제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신원확인을 할 수 있습니다. 기타 사전등록제와 관련한 자세한 내용은 경찰청 안전Dream(www.safe182.go.kr) 또는 실종아동찾기센터(☎182)에 문의하실 수 있습니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 사전등록제는 치매 노인이 길을 잃었을 경우를 대비하여, 경찰 시스템에 지문, 얼굴, 사진, 보호자의 연락처 등 정보를 미리 등록해 놓고, 실종시 등록된 자료를 활용하여 신속히 찾아주는 제도입니다. 보호자가 인터넷(안전Dream, www.safe182.go.kr)에서 직접 등록하거나, 관할 지역 경찰관서에 치매환자를 모시고 직접 방문해 언제든지 등록할 수 있습니다. 길을 잃거나 보호자가 확인되지 않는 치매환자를 경찰에서 보호 시, 이전에는 보호자의 실종 신고가 있어야 신원을 확인할 수 있었지만, 지문 등 사전등록제도의 도입으로 실종 신고가 없더라도 사전등록된 정보와 지문 매칭, 사진(얼굴) 유사도 검색 등 첨단 기술을 활용해 신원확인을 할 수 있습니다. 기타 사전등록제와 관련한 자세한 내용은 경찰청 안전Dream(www.safe182.go.kr) 또는 실종아동찾기센터(☎182)에 문의하실 수 있습니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배회감지기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>만약 치매 노인이 안심 지역을 이탈할 경우 배회감지기는 무슨 역할을 하나요?</t>
+  </si>
+  <si>
+    <t>가족에게 알림 메시지를 전송하여 미연에 사고를 방지</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 배회감지기(GPS)란 위치추적장치(GPS)가 탑재되어 있어 치매 노인이 보호자를 이탈한 경우 보호자가 5분 단위로 노인의 위치를 실시간 조회할 수 있고, 보호자가 설정해놓은 안심지역 3곳을 이탈할 경우 가족에게 알림 메시지를 전송하여 미연에 사고를 방지할 수 있는 장치를 말합니다. 노인장기요양서비스 재가급여 수급자로서, 치매증상이 있거나 배회 등 문제행동을 보이는 노인이 이용할 수 있습니다. 치매 노인이 완전와상으로 스스로 전혀 움직이지 못하는 상태, 길 잃기 등 문제 행동을 보이지 않는 상태 또는 장기요양시설 입소한 경우에 배회감지기를 신청할 수 없습니다. 배회감지기는 수급자나 가족이 장기요양급여 인정서와 복지용구 급여확인서를 가지고 복지용구사업소에 방문하여 신청 가능합니다. 기기의 종류는 목에 걸고 다닐 수 있을 정도로 가볍고 작은 사이즈의 목걸이형과 침대 아래나 출입구에 설치해 밟고 지나가면 신호를 보내주는 매트형이 있습니다. 일반대상자는 15%, 경감대상자는 7.5%의 본인부담금이 있고, 기초생활수급자는 본인부담금 없이 이용가능합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>후견,제도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최근 치매판정을 받은 형의 자녀들이 재산분쟁에만 골몰하는 것을 봤어. 그래서 미리 후견인을 지정해 두는 제도가 있니?</t>
+  </si>
+  <si>
+    <t>임의후견제도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 치매 노인을 위한 후견 제도는 성년후견, 한정후견, 특정후견 그리고 임의후견이 있습니다. 성년후견 제도는 치매 등의 사유로 인한 정신적 제약으로 사무를 처리할 능력이 지속적으로 결여된 성인이 가정법원의 후견개시심판으로 선임된 후견인의 지원을 통해 보호를 받는 제도입니다. 예를 들어, 재산관리·요양원 입소가 필요한 치매 노인일 경우에 성년후견제도가 적용될 수 있습니다. 한정후견 제도는 치매 등의 사유로 인한 정신적 제약으로 사무를 처리할 능력이 부족한 성인이 가정법원의 후견개시심판으로 선임된 후견인의 지원을 통해 보호를 받는 제도입니다. 예를 들어, 어렵고 복잡한 일은 처리하기 어려운 초기 치매일 경우에 한정후견제도가 적용될 수 있습니다. 특정후견 제도는 치매 등의 사유로 인한 정신적 제약으로 일시적 후원 또는 특정한 사무에 관한 후원이 필요한 성인이 가정법원의 후견개시심판으로 선임된 후견인의 지원을 통해 보호를 받는 제도입니다. 예를 들어, 딸이 없는 한 달 동안만 도움을 받고 싶은 치매 노인일 경우에 특정후견제도가 적용될 수 있습니다. 임의후견 제도는 치매 등의 사유로 인한 정신적 제약으로 사무를 처리할 능력이 부족한 상황에 있거나 부족하게 될 상황에 대비하여 스스로 후견계약을 체결하여 자신의 재산관리 및 신상보호에 관한 사무의 전부 또는 일부를 후견인에게 위탁하고 그 위탁사무에 관하여 대리권을 수여하는 것을 내용으로 하는 제도입니다. 예를 들어, 미리 후견인을 지정해 두고 싶은 분일 경우에 임의후견제도가 적용될 수 있습니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>후견인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>치매 환자에 대한 후견인은 누가 될 수 있니?</t>
+  </si>
+  <si>
+    <t>가족(친족,친구,이웃), 전문가(법무사,변호사,세무사,사회복지사), 법인</t>
+  </si>
+  <si>
+    <t>치매 환자의 후견인가 수행할 수 있는 재산관리 업무 알려줘.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">부동산의 관리·보존·처분, 예금 및 보험 등의 관리, 정기적 수입 및 지출에 관한 관리, 물품의 구입·판매, 서비스 이용계약 체결·변경 ·종료, 유체동산, 증서 및 중요문서의 보관 및 관리, 공법상의 행위 (세무신고 등), 상속의 승인, 한정승인 또는 포기 및 상속재산의 분할에 관한 협의 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 본인, 배우자, 4촌 이내의 친족 등이 가정법원에 후견인을 청구할 수 있으며 가정법원의 결정을 거쳐 후견인이 선임됩니다. 청구권자가 성년후견 제도를 청구하면 가정법원의 결정을 거쳐 성년후견인이 선임됩니다. 성년후견인은 피성년후견인의 법률행위를 대리하고, 피성년후견인의 법률행위를 취소할 수 있습니다. 단, 일용품 구입 등 일상생활에 필요하고 대가가 과도하지 않은 법률행위는 취소할 수 없습니다.  청구권자가 한정후견 제도를 청구하면 가정법원의 결정을 거쳐 한정후견인이 선임됩니다. 한정후견인은 가정법원에서 정한 범위의 법률행위를 대리하거나, 가정법원이 정한 범위에서 후견인의 동의를 받지 않은 피후견인의 법률행위를 취소할 수 있습니다.  청구권자가 특정후견 제도를 청구하면 가정법원의 결정을 거쳐 특정후견인이 선임됩니다. 특정후견인은 일정 기간 또는 특정한 사무를 후원 또는 대리합니다.  청구권자가 임의후견 제도를 청구하면 가정법원과 임의 후견 감독인을 거쳐 임의후견인이 선임됩니다. 임의후견인은 후견계약을 통해 미리 정해둔 재산관리 및 신상보호업무 등 법률행위를 대리합니다. 후견인은 가족(친족,친구,이웃), 전문가(법무사,변호사,세무사,사회복지사), 법인이 될 수 있습니다. 후견인은 부동산의 관리·보존·처분, 예금 및 보험 등의 관리, 정기적 수입 및 지출에 관한 관리, 물품의 구입·판매, 서비스 이용계약 체결·변경 ·종료, 유체동산, 증서 및 중요문서의 보관 및 관리, 공법상의 행위 (세무신고 등), 상속의 승인, 한정승인 또는 포기 및 상속재산의 분할에 관한 협의 같은 재산관리를 수행합니다. 또한 후견인은 의료행위, 주거관련 행위 및 그 밖의 일상생활을 지원해야 합니다. 후견인에 대해 궁금한 점이 있다면 가정법원 및 지역 지방법원으로 직접 문의하면 됩니다. 직접 문의하지 못한다면 치매상담콜센터 ☎ 1899 – 9988로 문의하면 됩니다. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 본인, 배우자, 4촌 이내의 친족 등이 가정법원에 후견인을 청구할 수 있으며 가정법원의 결정을 거쳐 후견인이 선임됩니다. 청구권자가 성년후견 제도를 청구하면 가정법원의 결정을 거쳐 성년후견인이 선임됩니다. 성년후견인은 피성년후견인의 법률행위를 대리하고, 피성년후견인의 법률행위를 취소할 수 있습니다. 단, 일용품 구입 등 일상생활에 필요하고 대가가 과도하지 않은 법률행위는 취소할 수 없습니다.  청구권자가 한정후견 제도를 청구하면 가정법원의 결정을 거쳐 한정후견인이 선임됩니다. 한정후견인은 가정법원에서 정한 범위의 법률행위를 대리하거나, 가정법원이 정한 범위에서 후견인의 동의를 받지 않은 피후견인의 법률행위를 취소할 수 있습니다.  청구권자가 특정후견 제도를 청구하면 가정법원의 결정을 거쳐 특정후견인이 선임됩니다. 특정후견인은 일정 기간 또는 특정한 사무를 후원 또는 대리합니다.  청구권자가 임의후견 제도를 청구하면 가정법원과 임의 후견 감독인을 거쳐 임의후견인이 선임됩니다. 임의후견인은 후견계약을 통해 미리 정해둔 재산관리 및 신상보호업무 등 법률행위를 대리합니다. 후견인은 가족(친족,친구,이웃), 전문가(법무사,변호사,세무사,사회복지사), 법인이 될 수 있습니다. 후견인은 부동산의 관리·보존·처분, 예금 및 보험 등의 관리, 정기적 수입 및 지출에 관한 관리, 물품의 구입·판매, 서비스 이용계약 체결·변경 ·종료, 유체동산, 증서 및 중요문서의 보관 및 관리, 공법상의 행위 (세무신고 등), 상속의 승인, 한정승인 또는 포기 및 상속재산의 분할에 관한 협의 같은 재산관리를 수행합니다. 또한 후견인은 의료행위, 주거관련 행위 및 그 밖의 일상생활을 지원해야 합니다. 후견인에 대해 궁금한 점이 있다면 가정법원 및 지역 지방법원으로 직접 문의하면 됩니다. 직접 문의하지 못한다면 치매상담콜센터 ☎ 1899 – 9989로 문의하면 됩니다.</t>
+  </si>
+  <si>
+    <t>노인복지법에 의해 노인은 후손의 양육과 국가 및 사회의 발전에 기여하여 온 사람으로서 존경받으며 건전하고 안정된 생활을 보장받고, 그 능력에 따라 적당한 일에 종사하고 사회적 활동에 참여할 기회를 보장 받습니다. 또한, 보건복지부장관은 노인의 보건복지에 관한 실태조사를 3년마다 실시하고 그 결과를 공표해야 합니다. 노인에 대한 사회적 관심과 공경의식을 높이기 위해 매년 10월 2일을 노인의 날, 매년 10월을 경로의 달로 합니다. 부모에 대한 효사상을 높이기 위해 매년 5월 8일을 어버이날로 합니다. 범국민적으로 노인학대에 대한 인식을 높이고 관심을 유도하기 위해 매년 6월 15일을 노인학대예방의 날로 하고, 국가와 지방자치단체는 노인학대예방의 날의 취지에 맞는 행사와 홍보를 실시하도록 노력해야 합니다. 국가와 지방자치단체는 노인복지에 관해 주거·보건·소득·여가 및 안전·권익보호 등의 분야로 나누어 매년 노인보건복지 사업안내, 기초연금 사업안내 등을 발표하고 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보건복지부장관, 특별시장·광역시장·특별자치시장·도지사·특별자치도지사, 시장·군수·구청장은 노인복지를 위해 필요하다고 인정되는 때에는 65세 이상의 자 또는 그를 보호하고 있는 자를 관계 공무원 또는 노인복지상담원이 상담 및 지도해야 합니다. 그리고 65세 이상의 자로서 신체적·정신적·경제적 이유 또는 환경상의 이유로 거택에서 보호받기가 곤란한 자를 노인주거복지시설 또는 재가노인복지시설에 입소시키거나 입소를 위탁해야 합니다. 보건복지부장관, 시·도지사 또는 시장·군수·구청장은 65세 미만의 자에 대하여도 그 노쇠현상이 현저하여 특별히 보호할 필요가 있다고 인정할 때에는 위와 같은 조치를 할 수 있습니다. 보건복지부장관, 시·도지사 또는 시장·군수·구청장은 입소한 노인이 사망한 경우에 그 자에 대한 장례를 할 자가 없을 때에는 그 장례를 하거나 해당 시설의 장으로 하여금 그 장례를 하게 할 수 있습니다. 노인주거복지시설은 생계급여 또는 의료급여 수급자이거나 부양을 받지 못하는 등의 65세 또는 입소비용을 전액 부담하고 단독취사 등 독립생활이 가능한 60세 이상의 노인이 가정과 같은 주거공간에서 일상생활에 필요한 편의를 제공받을 수 있는 시설을 말합니다. 노인주거복지시설에는 양로시설, 노인공동생활가정, 노인복지주택이 있습니다. 양로시설이란 노인을 입소시켜 급식과 그 밖에 일상생활에 필요한 편의를 제공함을 목적으로 하는 시설입니다. 노인공동생활가정이란 노인들에게 가정과 같은 주거여건과 급식, 그 밖에 일상생활에 필요한 편의를 제공함을 목적으로 하는 시설입니다. 노인복지주택이란 노인에게 주거시설을 임대하여 주거의 편의·생활지도·상담 및 안전관리 등 일상생활에 필요한 편의를 제공함을 목적으로 하는 시설입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>노인복지시설의 입소 대상자는 생계급여 수급자 또는 의료급여 수급자로서 65세 이상의 사람, 부양의무자로부터 적절한 부양을 받지 못하는 65세 이상의 사람, 본인 및 본인과 생계를 같이 하고 있는 부양의무자의 1인당 월평균 소득액이 전년도의 도시근로자가구 1인당 월평균 소득액이하인 자로서 65세 이상의 사람, 양로시설 또는 노인공동생활가정의 경우일 때 60세 이상의 사람이 있습니다. 생계급여 수급자와 의료급여 수급자의 입소비용을 국가 및 지방자치단체에서 전액 부담합니다. 나머지 입소비용은 입소자 본인이 일부 혹은 전부 부담합니다. 생계급여 수급자, 의료급여 수급자, 부양의무자로부터 적절한 부양을 받지 못하는 노인이 양로시설 또는 노인공동생활가정에 들어가려는 경우에는 입소신청서에 입소신청사유서 및 관련 증빙자료를 첨부하여 주소지를 관할하는 특별자치시장·특별자치도지사·시장·군수·구청장에게 제출해야 합니다. 나머지 입소대상자가 양로시설 또는 노인공동생활가정에 들어가려는 경우에는 당사자간의 계약에 따릅니다. 노인복지주택의 입소대상자는 단독취사 등 독립된 주거생활을 하는 데 지장이 없는 60세 이상의 사람이며 입소비용을 전부 본인이 부담해야 합니다. 입소자의 배우자와 입소자격자가 부양을 책임지고 있는 19세 미만의 자녀·손자녀는 함께 입소할 수 있습니다. 노인복지주택을 임차한 사람은 해당 노인주거시설을 입소자격자가 아닌 사람에게 다시 임대할 수 없습니다. 입소자격자가 아닌 사람에게 임대한 사람은 1년 이하의 징역 또는 1천만원 이하의 벌금에 처해집니다. 노인복지주택에 들어가려는 사람은 임대차계약에 따릅니다. 이 경우 임대차계약 신청자가 해당 시설의 정원을 초과하는 때에는 다음의 순위에 따르되, 같은 순위자가 있는 때에는 신청순위에 따라 결정합니다. 신청순위는 1순위:부양의무자가 없는 사람, 2순위:주민등록법 상 연령이 많은 사람, 3순위:배우자와 함께 입소하는 사람, 4순위:19세 미만의 자녀·손자녀와 함께 입소하는 사람입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">노인의료복지시설은 노인성질환 등 심신의 상당한 장애로 요양이 필요한 65세 이상의 노인이 입소하여 급식·요양 그 밖의 일상생활에 필요한 편의를 제공받는 시설을 말합니다. 노인의료복지설의 종류는 노인요양시설과 노인요양공동생활가정이 있습니다. 노인요양시설은 치매·중풍 등 노인성질환 등으로 심신에 상당한 장애가 발생하여 도움을 필요로 하는 노인을 입소시켜 급식·요양과 그 밖에 일상생활에 필요한 편의를 제공함을 목적으로 하는 시설입니다. 노인요양공동생활가정은 치매·중풍 등 노인성질환 등으로 심신에 상당한 장애가 발생하여 도움을 필요로 하는 노인에게 가정과 같은 주거여건과 급식·요양, 그 밖에 일상생활에 필요한 편의를 제공함을 목적으로 하는 시설입니다. 노인의료복지시설의 입소대상자는 「노인장기요양보험법」 제15조에 따른 수급자, 생계급여 수급자, 의료급여 수급자, 부양의무자로부터 적절한 부양을 받지 못하는 65세 이상의 사람, 민간 노인요양시설 또는 노인요양공동생활가정의 경우 60세 이상의 사람입니다. 노인의료복지시설에 들어가려는 경우에는 입소신청서, 국가의료기관에서 발행한 건강진단서, 입소신청사유서 및 관련 증빙자료 각 1부를 제출해야 합니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>노인여가복지시설은 65세 또는 60세 이상의 노인들이 여가를 즐기고 친목도모·취미생활 등을 할 수 있는 시설을 말합니다. 노인여가복지시설의 종류는 노인복지관, 경로당, 노인교실이 있습니다. 노인복지관은 노인의 교양·취미생활 및 사회참여활동 등에 대한 각종 정보와 서비스를 제공하고, 건강증진 및 질병예방과 소득보장·재가복지, 그 밖에 노인의 복지증진에 필요한 서비스를 제공함을 목적으로 하는 시설입니다. 경로당은 지역노인들이 자율적으로 친목도모·취미활동·공동작업장 운영 및 각종 정보교환과 기타 여가활동을 할 수 있도록 하는 장소를 제공함을 목적으로 하는 시설입니다. 노인교실은 노인들에 대하여 사회활동 참여욕구를 충족시키기 위해 건전한 취미생활·노인건강유지·소득보장, 그 밖에 일상생활과 관련한 학습프로그램을 제공함을 목적으로 하는 시설입니다. 노인복지관 및 노인교실은 60세 이상 가능하고 경로당은 65세 이상 가능합니다. 위의 규정에도 불구하고 노인복지관 및 노인교실 이용대상자의 배우자는 60세 미만인 때에도 이용대상자와 함께 이용할 수 있습니다. 노인여가복지시설의 이용은 시설별 운영규정이 정하는 바에 따릅니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>노인여가복지시설은 65세 또는 60세 이상의 노인들이 여가를 즐기고 친목도모·취미생활 등을 할 수 있는 시설을 말합니다. 노인여가복지시설의 종류는 노인복지관, 경로당, 노인교실이 있습니다. 노인복지관은 노인의 교양·취미생활 및 사회참여활동 등에 대한 각종 정보와 서비스를 제공하고, 건강증진 및 질병예방과 소득보장·재가복지, 그 밖에 노인의 복지증진에 필요한 서비스를 제공함을 목적으로 하는 시설입니다. 경로당은 지역노인들이 자율적으로 친목도모·취미활동·공동작업장 운영 및 각종 정보교환과 기타 여가활동을 할 수 있도록 하는 장소를 제공함을 목적으로 하는 시설입니다. 노인교실은 노인들에 대하여 사회활동 참여욕구를 충족시키기 위해 건전한 취미생활·노인건강유지·소득보장, 그 밖에 일상생활과 관련한 학습프로그램을 제공함을 목적으로 하는 시설입니다. 노인복지관 및 노인교실은 60세 이상 가능하고 경로당은 65세 이상 가능합니다. 위의 규정에도 불구하고 노인복지관 및 노인교실 이용대상자의 배우자는 61세 미만인 때에도 이용대상자와 함께 이용할 수 있습니다. 노인여가복지시설의 이용은 시설별 운영규정이 정하는 바에 따릅니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">재가노인복지시설은 정신적·신체적인 이유로 독립적인 일상생활을 수행하기 곤란한 65세 또는 60세 이상의 노인과 노인 부양가정에 필요한 각종 서비스를 제공하는 시설을 말합니다. 재가노인복지시설의 서비스 종류는 방문요양서비스, 주·야간보호서비스, 단기보호서비스, 방문 목욕서비스, 방문간호서비스, 복지용구지원서비스가 있습니다. 방문요양서비스는 가정에서 일상생활을 영위하고 있는 노인(이하 '재가노인'이라 함)으로서 신체적·정신적 장애로 어려움을 겪고 있는 노인에게 필요한 각종 편의를 제공하여 지역사회안에서 건전하고 안정된 노후를 영위하도록 하는 서비스입니다. 주·야간보호서비스는 부득이한 사유로 가족의 보호를 받을 수 없는 심신이 허약한 노인과 장애노인을 주간 또는 야간 동안 보호시설에 입소시켜 필요한 각종 편의를 제공하여 이들의 생활안정과 심신기능의 유지·향상을 도모하고, 그 가족의 신체적·정신적 부담을 덜어주기 위한 서비스입니다. 단기보호서비스는 부득이한 사유로 가족의 보호를 받을 수 없어 일시적으로 보호가 필요한 심신이 허약한 노인과 장애노인을 보호시설에 단기간 입소시켜 보호함으로써 노인 및 노인가정의 복지증진을 도모하기 위한 서비스입니다. 방문 목욕서비스는 목욕장비를 갖추고 재가노인을 방문하여 목욕을 제공하는 서비스입니다. 재가노인지원서비스는 재가노인에게 노인생활 및 신상에 관한 상담을 제공하고, 재가노인 및 가족 등 보호자를 교육하며 각종 편의를 제공하여 지역사회 안에서 건전하고 안정된 노후생활을 영위하도록 하는 서비스입니다. 방문간호서비스는 간호사 등이 의사, 한의사 또는 치과의사의 지시서에 따라 재가노인의 가정 등을 방문하여 간호, 진료의 보조, 요양에 관한 상담 또는 구강위생 등을 제공하는 서비스입니다. 복지용구지원서비스는 장기요양기관이 수급자의일상생활·신체활동 지원 및 인지기능의 유지·향상에 필요한 복지용구를 제공하거나 대여하는 서비스입니다. </t>
+  </si>
+  <si>
+    <t>노인장기요양보험법 제15조에 따른 수급자는 재가노인복지시설을 이용할 수 있고 비용은 노인장기요양보험법령이 정하는 바에 따릅니다. 심신이 허약하거나 장애가 있는 65세 이상의 자는 누구나 재가노인복지시설을 이용할 수 있습니다. 재가노인복지시설을 이용할 때 생계급여 수급자, 의료급여 수급자, 부양의무자로부터 적절한 부양을 받지 못하는 사람은 국가 및 지방자치단체에서 전액을 부담하고 나머지는 이용자 본인이 전액을 부담합니다. 재가노인복지시설의 이용은 당사자간 계약에 따릅니다. 방문요양서비스는 1일 중 일정시간 동안 가정에서의 보호가 필요한 사람이 이용할 수 있습니다. 주·야간보호서비스 : 주간 또는 야간 동안의 보호가 필요한 사람이 이용할 수 있습니다. 단기보호서비스은 월 1일 이상 15일 이하 단기간의 보호가 필요한 사람이 이용할 수 있습니다. 방문 목욕서비스은 가정에서의 목욕이 필요한 사람이 이용할 수 있습니다. 재가노인지원서비스은 위 가.부터 라.까지의 서비스 이외의 서비스로서 상담·교육 및 각종 지원 서비스가 필요한 사람이 이용할 수 있습니다. 방문간호서비스은 가정 등에서 간호, 진료의 보조, 요양에 관한 상담 또는 구강위생 등이 필요한 사람이 이용할 수 있습니다. 복지용구지원서비스은 복지용구가 필요한 사람이 이용할 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">국가 또는 지방자치단체는 홀로 사는 노인에 대하여 방문요양과 돌봄 등의 서비스와 안전확인 등의 보호조치를 취해야 합니다. 노인맞춤돌봄서비스란 일상생활 영위가 어려운 취약노인에게 적절한 돌봄서비스를 제공하여 안정적인 노후생활 보장, 노인의 기능건강 유지 및 악화를 예방하기 위한 방문형, 통원형(집단 프로그램) 등의 직접 서비스 및 연계 서비스(민간후원 자원), 특화서비스, 사후관리 서비스 등을 말합니다. 노인맞춤돌봄서비스는 다른 보건복지 서비스의 혜택을 받지 못하는 사람들에게 최소한의 사회 복지 서비스를 제공해 주기 위해 마련된 복지 서비스 중의 하나입니다. 그렇기 때문에 장기요양급여를 받고 있는 사람들은 노인돌봄기본서비스 대상자에서 제외됩니다. 65세 이상 국민기초생활수급자, 차상위계층 또는 기초연금수급자로서 유사 중복사업 자격에 해당되지 않는 사람만 노인맞춤돌봄서비스를 받을 수 있습니다. 예를 들어, 독거·조손·고령부부 가구 노인 등 돌봄이 필요한 노인은 노인맞춤돌봄서비스를 이용할 수 있습니다. 또는 신체적 기능, 저하정신적 어려움(인지저하, 우울감 등) 등으로 돌봄이 필요한 노인 고독사 및 자살 위험이 높은 노인 등과 같은 사람들이 노인맞춤돌봄서비스를 이용할 수 있습니다. 노인맞춤돌봄서비스를 이용하고 싶다면 중점돌봄군과 일반돌봄군에 해당해야 합니다. 중점돌봄군은 신체적인 기능제한으로 일상생활지원 필요가 큰 대상으로 대상자 선정조사 결과, ‘신체’영역이 ‘상’이면서 ‘사회’영역 또는 ‘정신’영역에서 ‘중’ 또는 ‘상’이 1개 이상으로 판정된 대상자이여야 합니다. 일반돌봄군은 사회적인 관계 단절 및 일상생활의 어려움으로 돌봄이 필요가 있는 대상으로 대상자 선정조사 결과, ‘사회’영역이 ‘중’이상 이면서, ‘신체’영역 또는 ‘정신’영역에서 ‘중’ 또는 ‘상’이 1개 이상으로 판정된 대상자입니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">노인맞춤돌봄서비스는 방문형, 통원형(집단 프로그램) 등의 직접 서비스 및 연계 서비스 제공합니다. 노인맞춤돌봄서비스의 종류에는 직접 서비스, 연계 서비스, 특화 서비스, 사후관리 서비스가 있습니다. 직접 서비스는 상자의 전반적인 안전 여부를 점검하기 위하여 생활환경, 가구구조와 같은 환경 여건 뿐만 아니라 노인의 기본적인 신체적 정신적 사회적 안녕 여부 등을 점검 지원하는 서비스, 대상자가 사회적 관계망을 형성·확장하여 사회적 교류와 활동을 유지하도록 지원하는 서비스, 사회적, 신체적, 정신적 기능을 유지하거나 악화를 지연·예방하기 위한 교육·프로그램을 제공하는 서비스, 대상자의 일상생활을 지원하기 위하여 외출동행, 가사지원을 제공하는 서비스를 말합니다. 직접 서비스의 예시로는 안전안부확인(방문전화 ICT), 생활안전점검, 정보제공, 말벗, 사회관계 향상 프로그램, 자조모임, 신체건강정신건강분야 생활교육, 이동활동지원, 가사지원이 있습니다. 연계 서비스는 대상자의 안정적인 생활을 지원하기 위하여 지역사회 내 민간자원 등의 후원물품 이나 서비스를 연계 지원하는 서비스입니다. 연계 서비스를 수행하는 기관은 물품후원, 자원봉사자 등 민간후원자원을 적극 발굴연계하고  생활지원연계, 주거개선연계, 건강지원연계, 기타 서비스 등을 제공합니다. 특화 서비스는 은둔형우울형 노인을 대상으로 척도(우울감, 자살생각, 고독감 등) 등을 활용하여 개별 맞춤형 상담 및 집단활동 제공합니다. 사후관리 서비스는 사후관리가 필요한 대상자에게 정기적인 모니터링 및 자원연계 실시하는 서비스입니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>노인맞춤돌봄서비스의 절차는 서비스 신청 접수, 대상자 선정조사 및 서비스 상담, 서비스 제공계획 수립, 승인 요청, 심의 및 결정, 서비스 제공, 재사정, 종결 및 사후관리 순으로 진행됩니다. 먼저 노인맞춤돌봄서비스를 필요로 하는 노인 또는 그 가족 등이 읍면동 주민센터 방문 등을 통해 노인맞춤돌봄 서비스를 신청합니다. 읍면동 담당공무원은 신청자의 나이, 소득, 유사중복 서비스 수혜 여부 등 신청자격을 확인 후 접수하고 결과를 수행기관에 통보합니다. 전담사회복지사 등은 서비스 신청자(또는 대상자)의 가정 방문 등을 통해 선정조사 및 서비스 상담을 실시합니다. 전담사회복지사는 대상자 선정조사 결과에 따라 대상자 자격기준에 해당되는 경우에 한해 서비스 내용, 서비스 방법, 제공빈도, 담당 생활지원사 배정 등을 포함한 구체적인 서비스 제공계획을 수립합니다. 수행기관은 대상자 선정조사 결과 및 서비스 제공계획을 시군구에 결정을 요청합니다. 시군구는 노인맞춤돌봄서비스심의회 등을 통해 대상자 선정 및 서비스 제공계획의 적합성, 적절성, 타당성 등을 심의하여 승인 여부 등을 결정하고 그 결과를 수행기관에 통보한 뒤 신청자에게 서비스 결정을 통지합니다. 서비스 제공기간은 서비스 승인 익일부터 1년입니다. 다만, 긴급한 돌봄이 필요한 경우에는 심의 전부터 서비스 제공기간을 시작(책정요청일을 별도로 둠)하여 사후 심의를 거칠 수 있습니다. 서비스 이용자의 욕구와 상태 등에 맞는 적절한 서비스가 제공되고 있는지 재사정함으로써 제공기간 종료 3개월 이내 서비스 제공여부를 다시 결정합니다. 마지막으로 사망, 시설 입소, 서비스 거부 등의 사유로 서비스 종결이 필요할 경우 사례실무회의 및 시군구 승인을 통해 종결처리 및 사후관리가 실시됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">노인맞춤돌봄서비스가 종결되면 1년 내로 수행기관에서 사후관리 서비스를 제공합니다. 사후관리 주체는 생활지원사이고, 전담사회복지사는 자원연계 등의 지원을 합니다. 노인맞춤돌봄서비스 종결자 중 사후관리가 필요한 경우로서 이용자가 장기요양등급을 인정받아 재가장기요양서비스를 이용하게 되었을 때 원활한 서비스 이용적응을 모니터링하고 필요한 물품 등의 연계하는 등 사후 관리 필요한 경우에 사후관리 대상으로 합니다. 기존 사회 자원연계 사업 대상자 중 장기요양 등급자가 사후관리 대상이 됩니다. 사후관리 방법은 안부확인 및 모니터링을 실시하고 반기별 1회 이상 방문 및 분기별 1회 이상 유선통화를 실시합니다. 그리고 필요시 자원연계서비스를 제공하며 기존 지역사회 자원연계 사업 대상자의 경우 자원연계서비스를 제공해야 합니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>특화서비스의 대상은 가족, 이웃 등과의 접촉이 거의 없어 고독사 및 자살위험이 높은 만 65세 이상 노인이며, 특화서비스 참여자 특성에 따라 은둔형, 우울형으로 운영(참여자는 수행기관당 최소 50명 이상, 은둔형은 최소 5명이상)합니다. 또한 고독사 및 자살위험이 크다고 판단되는 경우 자문위원단의 승인 후에 60세 이상으로 하향 조정을 할 수 있습니다. 먼저 특화서비스 전담사회복지사는 노인맞춤돌봄서비스 수행기관으로부터 특화서비스 제공이 필요한 자에 대한 서비스 의뢰서를 접수합니다. 특화서비스 전담사회복지사는 기존 대상자, 신규로 서비스에 의뢰된 자의 가정방문 등을 통해 서비스 이용자 선정을 위한 초기상담 및 척도검사를 실시합니다. 척도는 가족, 이웃 등과 관계가 단절되어 있으면서, 국민기초생활보장제도의 생계비, 의료비 수급 이외 공식·비공식 서비스를 이용하지 않는 노인에 해당하는 은둔형 집단과 자살시도 후 생존자 또는 우울증 진단을 받고 자살시도 가능성이 높은 노인에 해당하는 우울형 집단으로 나뉩니다. 특화서비스 전담사회복지사가 특화서비스 이용기준에 적합한 자 및 특화서비스 이용기준에 적합하지 않으나 자문위원단의 승인을 받아 서비스 이용자로 승인된 자를 대상으로 서비스 제공계획을 수립하여 서비스를 제공합니다. 은둔형 집단일 경우,  특화 서비스는 개별접근을 핵심방법론으로 하여 개인별 상담(25회기 이상)을 진행하며 집단접근도 활용할 수 있으나 참여도가 낮고 거부적 태도를 보일 수 있으므로 가급적 집단접근은 지양합니다. 우울형 집단일 경우, 특화 서비스는 개인별 상담(8회기 이상), 집단사회복지실천방법론에 의한 집단활동(수행기관 자체 개발 프로그램, 자조모임, 나들이 등), 의학적 접근(집단치료)을 핵심방법론으로 서비스를 제공합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>65세 이상의 의료급여 수급권자는 노인 건강검진을 2년에 1회 이상 국·공립병원, 보건소 또는 노인전문병원, 요양기관 및 의료급여기관에서 건강검진을 받을 수 있습니다. 시·군·구 관할 구역에 거주하는 65세 이상 의료급여 수급권자 중 노인 건강검진 희망자는 누구나 건강검진을 받을 수 있습니다. 건강보험 가입자의 경우에 ‘국민건강보험공단’의 건강검진을 받을 수 있습니다. 의료급여 수급권자는 66세가 되는 해에 생애전환기 건강검진을 받을 수 있습니다. 보건복지부장관, 특별시장·광역시장·특별자치시장·도지사·특별자치도지사 또는 시장·군수·구청장이 건강검진을 실시하려는 때에는 그 실시기간·실시장소·진단기관 및 대상자의 범위 등을 정하여 건강검진 실시 예정일 14일 전까지 이를 공고해야 합니다. 건강검진은 1차 및 2차 진단으로 구분하여 실시하고 있으며, 1차 건강검진은 1차 건강검진 항목을 대상으로 실시합니다. 2차 건강검진은 1차 진단결과 유소견자 및 전년도 진단결과 유질환자에 한하여 해당 질환별로 실시합니다. 주의할 점은 전년도 진단결과 유질환자는 1차 및 2차 건강검진을 동시에 받습니다. 건강검진 후 질환이 발견된 노인은 보건소의 등록관리 및 공공의료기관과의 연계를 통해 방문건강관리 또는 의료서비스를 체계적으로 제공받습니다. 성매개감염병 질환이 있는 노인은 보건소에서 무료로 치료를 받을 수 있습니다. 치매가 의심되는 노인은 무료 치매조기검진을 받을 수 있고 치매를 진단받은 경우 보건소의 치매안심센터에 등록되어 치매치료제 복용에 대한 치료비 지원을 받을 수 있습니다. 노인 건강검진 대상자는 보건소와 연계하여 무료 안검진과 개인수술비 지원을 받을 수 있습니다. 치과진료가 필요한 노인은 보건소의 구강보건센터와 연계하여 진료를 받을 수 있습니다.</t>
+  </si>
+  <si>
+    <t>60세 이상의 노인은 안질환을 조기에 발견하고 적기에 치료하여, 노인들의 실명 예방 및 일상생활이 가능하도록 무료로 눈 건강검진을 받을 수 있습니다. 눈 검진은 검진 사업 신청지역에 사는 60세 이상의 어르신이라면 누구나 참여가 가능합니다. 검진을 받으러 갈 때 신분증, 건강보험카드, 전화번호를 준비해야 합니다. 검진할 때, 정밀 안저검사, 안압검사, 굴절검사, 조절검사,각막곡률검사 등을 받을 수 있습니다. 검진을 받을 수 있는 시간은 검진을 받으려는 당일 접수를 하면 바로 받으실 수 있고, 오전 9시 30분부터 오후 3시까지 검진 접수를 할 수 있습니다.노인 건강검진 사업은 보건복지부와 함께 한국실명예방재단에서 시행하고 있습니다. 매년 1 ~ 2월경에 시·도에서 전국 보건소를 통해 검진 수요조사를 실행하고 희망 지역을 대상으로 일정을 계획하여 건강검진을 진행하고 있습니다. 단, 1일 검진 예상인원이 최소 100명 이상일 경우 신청이 가능하고, 농어촌 및 안과 접근이 낮은 지역을 우선 순위로 실시하며 환자 개별적 신청을 받지 않고 있으니 주의해야 합니다. 60세 이상 노인이거나 백내장, 망막질환, 녹내장 등 그 밖에 안질환을 진단받은 노인은 개안수술비를 지원받을 수 있습니다. 수술비 지원 신청 접수는 보건소에서 연중 수시로 받고 있습니다. 수술비를 신청할 때는 안 질환 의료지원 신청서, 안과 진료소견서(수술병원의 진단서), 기초생활수급자 및 차상위계층 증명서 1부, 한부모가족증명서 1부를 제출해야합니다. 수술비 지원 대상자 선정에는 1달 정도의 기간이 소요되며, 지원결정 통보 전에 수술을 받으면 지원을 받을 수 없으므로 대상자 선정 여부를 꼭 확인해야 합니다. 지원받을 수 있는 수술비의 범위는 초음파검사비 등의 사전검사비 1회, 수술비, 수술관련 재료비 등 개안수술비 총액 중에서 본인부담액 전액을 지원받을 수 있습니다. 수술비는 개안수술을 실시한 의료기관이 직접 한국실명예방재단에 청구하면 의료기관의 은행계좌에 바로 입금됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정부에서는 치매관리종합계획을 수립하여 이 계획에 따라 치매를 조기에 발견하기 위한 검진사업을 6개월을 주기로 시행하고 있습니다. 이에 따라 치매의 위험이 높은 60세 이상의 노인은 치매검진을 받고 치매를 조기에 발견하고 관리할 수 있습니다. 건강보험가입자 및 피부양자와 의료급여수급자는 치매 건강검진을 받을 수 있습니다. 검진은 치매 가능성이 높은 대상자를 가려내기 위한 선별검사와 치매진단을 위한 정밀검사로 구분되어 실시됩니다. 치매 조기검진을 통해 치매, 치매고위험군, 정상 중 한 가지로 판정을 받거나 전문의료기관에서 이미 치매로 진단을 받은 대상자는 보건소에 설치된 치매상담센터에 등록되어 각 구분에 따라 치매 관리 서비스, 치매고위험군 관리 서비스, 정상 관리 서비스를 받습니다. 치매 관리 서비스는 인지건강센터 프로그램 시행, 방문간호, 조호물품 제공, 배회가능어르신 인식표 보급, 치매관련 정보 제공, 가족모임, 지역 치매관련 자원연계(의료기관,복지시설 등 연계), 치료비 지원(저소득층) 등을 제공합니다. 치매고위험군 관리 서비스는 정기 정밀검진 서비스, 인지건강센터 프로그램 시행, 치매예방 정보제공 서비스, 치매예방 관련 프로그램 연계 서비스 등을 제공합니다. 정상 관리 서비스는 정기 선별검진 서비스, 치매예방 정보제공 서비스, 치매예방 관련 프로그램 연계 서비스 등을 제공합니다. 국가와 지방자치단체는 치매환자의 경제적 부담능력을 고려하여 치매 치료 및 진단에 드는 비용을 지원할 수 있습니다. 건강보험가입자, 피부양자, 의료급여수급권자 중 치매환자 중에서 소득이 기준 중위소득 120% 이하인 사람은 의료비를 지원받을 수 있습니다. 치매 치료를 위한 진료비와 진료시 처방받은 약제비에 대한 보험급여분 중 본인부담금에 대해 월 3만원(연간 36만원) 한도 내에서 지원받습니다. 치매환자 의료비를 지원받으려는 사람은 지원신청서, 통장 사본, 당해연도에 발행된 치매치료제가 포함된 약처방전 또는 약국 영수증을 관할 보건소장에게 제출해야 합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">노인이 후손의 양육과 국가 및 사회의 발전에 이바지하여 온 점을 고려하여 생활이 어려운 노인에게 생활안정을 지원하고 복지를 증진하기 위해 기초연금(이하 “연금”이라 함)을 지급합니다. 65세 이상인 본인 및 배우자의 소득인정액이 137만원(단독가구) 또는 219.2만원(부부가구) 이하인 노인은 기초연금을 받을 수 있습니다. 국민연금 수급자는 기초연금을 받을 수 있습니다. 기초연금의 소득인정액 요건 등을 충족하면 기초연금을 받을 수 있고, 국민연금액과 국민연금 가입기간이 반영된 국민연금 소득재분배급여(A급여) 등에 따라 기초연금액을 결정합니다. 또한 기초생활보장 수급자는 기초연금을 받을 수 있습니다. 다만, 기초연금 지급액을 소득으로 인정하기 때문에 기초생활보장 급여에 영향을 미칠 수도 있습니다. 기초생활보장제도는 ‘최후의 사회 안전망’으로 본인의 소득과 재산, 부양의무자의 지원, 기초연금을 포함한 여러 지원제도에도 불구하고 소득인정액이 최저생계비에 미달할 경우에, 그 차액을 지원해드리는 제도이기 때문입니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기초연금을 지급받으려는 사람 또는 그 친족, 그 밖의 관계인은 특별자치시장·특별자치도지사·시장·군수·구청장에게 기초연금의 지급을 신청할 수 있습니다. 본인이 직접 신청하시는 것이 원칙이나, 불가피할 경우 배우자나 자녀, 형제·자매, 친족, 사회복지시설장이 대리 신청할 수 있습니다. 대리인이 신청할 경우 본인 신분증 이외에 대리인의 신분증·위임장을 지참하셔야 합니다. 위임장 서식은 읍·면사무소 및 동 주민센터, 국민연금공단 지사에 구비되어 있으며, 보건복지부 기초연금 홈페이지(http://basicpension.mohw.go.kr)에서도 다운로드하실 수 있습니다. 기초연금의 지급을 신청하려는 사람은 연금지급신청서, 소득/재산 신고서, 금융정보의 제공 동의서면과 신분증을 특별자치시장·특별자치도지사·시장·군수·구청장에게 제출하여야 합니다. 신청인은 특별자치시장·특별자치도지사·시장·군수·구청장이 연금지급신청서를 접수한 날부터 30일 이내에 결정결과를 통지받습니다. 다만, 소득·재산 등의 조사에 시일을 필요로 하는 특별한 사유가 있는 경우에는 그 사유를 명시하여 접수한 날부터 60일 이내에 통지할 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기초연금 수급자는 지급 정지의 사유가 소멸한 경우, 기초연금 수급권 상실의 사유가 있는 경우, 기초연금 수급자 또는 그 배우자의 소득·재산의 변동이 발생한 경우, 기초연금 수급자가 결혼 또는 이혼을 하거나 그 배우자가 사망한 경우, 기초연금의 지급계좌 변경시 그리고 국민연금법에 따른 자격 및 국민연금으로 지급받는 금액의 변동의 경우에는 30일 이내에 그 사실을 특별자치시장·특별자치도지사·시장·군수·구청장에게 신고해야 합니다.  다만, 수급자가 사망한 경우에는 가족관계의 등록 등에 관한 법률 제85조에 따른 신고의무자가 특별자치시장·특별자치도지사·시장·군수·구청장에게 신고해야 합니다. 수급자는 변경신고를 하려면 변경신고서, 변경 내용을 확인할 수 있는 서류 그리고 신분증을 제출해야 합니다. 신청인은 특별자치시장·특별자치도지사·시장·군수·구청장이 변경신고서를 접수한 날부터 30일 이내에 결정결과를 통지받습니다. 다만, 변경된 소득·재산 등의 조사에 시일을 필요로 하는 특별한 사유가 있는 경우에는 그 사유를 명시하여 접수한 날부터 60일 이내에 통지할 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기초연금액은 기준연금액과 국민연금 급여액 등을 고려하여 산정합니다. 2020년도 기초연금액은 25만4천7백6십원이고 2021년도 기초연금액은 30만원입니다. 저소득층 기초연금 수급권자의 기준연금액은 30만원으로 합니다. 다만, 2020년 12월 31일까지 한시적으로 적용됩니다. 매년 고시하는 기준연금액의 적용기간은 해당 조정연도 1월부터 12월까지로 합니다. 수급권자 중 노령연금 수급권자, 분할연금 수급권자 그리고 국민연금 수급권자에게 지급하는 기초연금액은 기준연금액에서 소득재분배급여금액에 3분의 2를 곱한 금액을 뺀 후 부가연금액을 더한 금액을 산정합니다. 소득재분배급여란 국민연금 급여액 중 기초연금적 성격을 가진 부분으로, 개인별 기초연금액을 결정하는 기준이 되는 급여입니다. 소득재분배급여는 가입기간이 길수록, 일찍 가입할수록 소득재분배급여가 증가합니다. 또한 가입기간이 동일하더라도 가입시기, 가입이력에 따라 다를 금액을 다를 수 있습니다. 수급권자는 기초연금액을 연금의 지급을 신청한 날이 속하는 달부터 수급권을 상실한 날이 속하는 달까지 매월 정기적으로 지급받습니다. 연금은 매월 25일(지급일이 토요일·공휴일인 경우에는 그 전날에 지급)에 금융기관 또는 우편관서의 수급자 명의의 계좌(부부가 모두 수급자인 경우로서 배우자 일방이 지정하는 계좌를 포함)에 입금하는 방법으로 지급됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>본인과 그 배우자가 모두 기초연금 수급권자인 경우에는 각각의 기초연금액에서 기초연금액의 100분의 20에 해당하는 금액을 제외해야 합니다. 소득인정액과 기초연금액을 합산한 금액이 선정기준액 이상인 경우에는 선정기준액을 초과하는 금액의 범위에서 기초연금액의 일부를 감액할 수 있습니다. 소득인정액이란 본인 및 배우자의 소득평가액과 재산의 소득환산액을 합산한 금액을 말합니다. 선정기준액이란 연금 지급대상자의 선정기준이 되는 일정 금액을 말하며, 2020년 선정기준액은 배우자가 없는 노인가구의 경우 월 소득인정액 148만원, 배우자가 있는 노인가구의 경우 월 소득인정액 236.8만원입니다. 만약 소득인정액이 120만원인 어르신이 250,000원의 기초연금을 받으신다면, 기초연금을 못 받으시는 소득인정액이 137만원인 어르신보다 오히려 소득이 많아지게 됩니다. 이렇게 기초연금 수급으로 인해 발생할 수 있는 불공평성 문제를 해결하기 위해, 소득인정액과 기초연금 산정액을 합한 금액이 선정기준액 이상인 경우 기초연금액의 일부를 감액합니다. 저소득 기초연금 수급자의 소득인정액과 기초연금액을 합산한 금액이 저소득자 선정기준액과 기준연금액을 합산한 금액 이상인 경우에는 저소득 기초연금 수급권자의 기초연금액에서 그 초과분을 뺀 금액을 지급합니다. 위에도 불구하고 본인 및 배우자가 모두 저소득 기초연금 수급권자로서 본인 및 배우자의 소득인정액과 「기초연금법」 제8조제1항에 따라 감액한 본인 및 배우자의 기초연금액을 합산한 금액을 모두 더한 금액이 저소득자 선정기준액과 「기초연금법」 제5조의2에 해당하지 않는 기초연금 수급권자의 기준연금액에 100분의 160을 곱한 금액을 더한 금액을 초과하는 경우에는 해당 본인 배우자의 기초연금액을 합산한 금액에서 그 초과분을 뺀 금액을 지급합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수급자가 사망한 경우 수급자에게 아직 지급되지 않은 연금이 있을 때에는 미지급 연금을 청구할 수 있습니다. 미지급 연금은 수급자의 사망 당시 생계를 같이 한 부양의무자(배우자와 직계혈족 및 그 배우자를 말함)가 신청해야지 자격 요건을 충족합니다. 미지급 연금의 지급을 청구할 수 있는 부양의무자의 지급 청구순위는 배우자, 자녀와 그 배우자, 부모, 손자녀와 그 배우자의 순으로 합니다. 미지급 연금을 받으려는 사람은 사망한 수급자의 주소지를 관할하는 특별자치시장·특별자치도지사·시장·군수·구청장에게 미지급연금지급청구서, 수급자의 사망사실을 입증할 수 있는 서류, 미지급 연금을 청구할 수 있는 부양의무자의 지급 청구순위와 부양의무자임을 확인할 수 있는 서류 그리고 신분증을 제출해야 합니다. 미지급 기초연금의 지급 청구를 받은 특별자치시장·특별자치도지사·시장·군수·구청장은 미지급 기초연금 지급 청구서를 접수한 날부터 7일 이내에 미지급 기초연금의 지급 여부를 청구인에게 통지해야 합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기초연금 지급의 결정이나 그 밖에 「기초연금법」에 따른 처분에 이의가 있는 사람은 특별자치시장·특별자치도지사·시장·군수·구청장에게 이의신청을 할 수 있습니다. 이의신청은 그 처분이 있음을 안 날부터 90일 이내에 서면으로 해야 합니다. 다만, 정당한 사유로 인하여 그 기간 이내에 이의신청을 할 수 없었음을 증명한 때에는 그 사유가 소멸한 때부터 60일 이내에 이의신청을 할 수 있습니다. 이의신청을 하려는 사람은 이의신청서, 이의신청의 내용을 확인할 수 있는 서류 그리고 신분증을 주소지를 관할하는 특별자치시장·특별자치도지사·시장·군수·구청장에게 제출해야 합니다. 신청인은 이의신청을 접수한 날부터 30일 이내에 특별자치시장·특별자치도지사·시장·군수·구청장의 이의신청 각하 또는 기각, 취소 또는 변경에 대한 결과를 통지받습니다. 다만, 소득·재산 등의 조사에 시일이 걸리는 등 특별한 사유가 있는 경우에는 그 사유를 명시하여 접수한 날부터 60일 이내에 결정·통지를 받을 수 있습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기초연금을 받은 사람이 거짓이나 그 밖의 부정한 방법으로 기초연금을 받은 경우에 지급한 기초연금액에 3년 만기 정기예금 이자율을 적용하여 계산한 이자를 붙여 반환해야 합니다. 또한 기초연금의 지급이 정지된 기간에 대하여 기초연금이 지급된 경우나 그 밖의 사유로 기초연금이 잘못 지급된 경우에 지급받은 기초연금액을 일시에 전액 반환해야 합니다. 특별자치시장·특별자치도지사·시장·군수·구청장은 환수할 기초연금액의 환수 대상자에게 지급할 기초연금액이 있는 경우 그 지급할 기초연금액을 환수할 기초연금액과 상계할 수 있습니다. 부당이득금을 납부하지 않을 때에는 지방세 체납처분의 예에 따라 징수됩니다. 다만, 부당이득을 환수할 권리와 수급권자의 권리는 5년간 행사하지 않으면 시효의 완성으로 소멸됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수급자가 금고 이상의 형을 선고받고 교정시설 또는 치료감호시설에 수용되어 있는 경우 혹은 수급자가 행방불명되거나 실종되는 등 사망한 것으로 추정되는 경우에는 그 사유가 발생한 날이 속하는 달의 다음 달부터 그 사유가 소멸한 날이 속하는 달까지는 기초연금을 지급 받지 못합니다.  수급자가 행방불명, 실종 또는 가출 등으로 경찰서 등 관계 행정기관에 신고가 접수된 날부터 보건복지부장관이 정하는 기간까지 생사를 확인할 수 없는 경우에는 그 기간이 만료한 때에 사망한 것으로 추정합니다. 수급자의 국외 체류기간이 60일 이상 지속되는 경우, 국외 체류 60일이 되는 날을 지급 정지의 사유가 발생한 날로 봅니다. 수급자가 「주민등록법」 제20조 제6항에 따라 거주불명자로 등록된 경우에 지급이 정지됩니다. 다만, 수급자의 실제 거주지를 알 수 있는 경우에는 그렇지 않습니다. 수급권자는 사망, 국적 상실, 국외 이주, 기초연금 수급권자에 해당하지 않게 된 때에 기초연금 수급권을 상실합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장기요양보험,장기요양급여</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장기요양보험이란 고령이나 노인성 질병 등의 사유로 일상생활을 혼자서 수행하기 어려운 노인 등에게 신체활동 또는 가사활동 지원 등의 장기요양급여를 제공하는 사회보장제도를 말합니다. 장기요양급여란 고령이나 노인성 질병 등의 사유로 6개월 이상 동안 혼자서 일상생활을 수행하기 어렵다고 인정되는 노인 등에게 신체활동·가사활동의 지원 또는 간병 등의 서비스나 이에 갈음하여 지급하는 현금 등을 말합니다. 장기요양보험의 가입자(이하 “장기요양보험가입자”라 함)는 「국민건강보험법」 제5조 및 제109조에 따른 가입자를 말합니다. 국민건강보험 가입자는 장기요양보험의 가입자가 됩니다. 즉, 장기요양보험만 별도로 가입할 수 있는 것이 아닙니다. 국민건강보험에 가입하게 되면 동시에 장기요양보험에도 강제로 가입되어 모든 국민건강보험 가입자는 장기요양보험 가입자가 되는 것입니다. 그래서 장기요양보험료도 ‘건강보험료x장기요양보험료율’로 산정하여 국민건강보험료와 통합하여 납부하면 됩니다. 외국인은 장기요양보험을 가입할 수 없습니다. 하지만 직장가입자가 된 외국인이거나 「출입국관리법」 제10조에 따라 산업연수활동을 할 수 있는 체류자격을 가지고 지정된 사업체에서 연수하고 있는 외국인이면 예외적으로 장기요양보험에 가입할 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장기요양급여에는 재가급여, 시설급여, 특별현금급여가 있습니다. 재가급여의 종류는 방문요양, 방문목욕, 방문간호, 주·야간보호, 단기보호 등이 있습니다. 방문요양은 장기요양요원이 수급자의 가정 등을 방문하여 신체활동 및 가사활동 등을 지원하는 급여입니다. 방문목욕은 장기요양요원이 목욕설비를 갖춘 장비를 이용하여 수급자의 가정 등을 방문하여 목욕을 제공하는 급여입니다. 방문간호는 장기요양요원인 간호사 등이 의사, 한의사 또는 치과의사의 지시서에 따라 수급자의 가정 등을 방문하여 간호, 진료의 보조, 요양에 관한 상담 또는 구강위생 등을 제공하는 급여입니다. 주·야간보호란 수급자를 하루 중 일정한 시간 동안 장기요양기관에 보호하여 신체활동 지원 및 심신기능의 유지·향상을 위한 교육·훈련 등을 제공하는 급여입니다. 단기보호란 수급자를 월 9일 이내에 일정 기간 동안 장기요양기관에 보호하여 신체활동 지원 및 심신기능의 유지·향상을 위한 교육·훈련 등을 제공하는 급여입니다. 그 밖의 재가급여로는 수급자의 일상생활·신체활동지원 및 인지기능의 유지·향상에 필요한 용구를 제공하거나 가정을 방문하여 재활에 관한 지원 등을 제공하는 급여입니다. 시설급여는 장기요양기관에 장기간 입소한 수급자에게 신체활동 지원 및 심신기능의 유지·향상을 위한 교육·훈련 등을 제공하는 급여를 말합니다. 특별현금급여의 종류는 가족요양비, 특례요양비 그리고 요양병원간병비가 있습니다. 가족요양비는 섬 등 요양기관이 현저히 부족한 지역에 거주하는 수급자가 가족 등으로부터 방문요양에 상당한 장기요양급여를 받은 경우 국민건강보험공단에서 해당 수급자에게 지급하는 급여입니다. 특례요양비는 수급자가 장기요양기관이 아닌 노인요양시설 등의 기관 또는 시설에서 재가급여 또는 시설급여에 상당한 장기요양급여를 받은 경우 공단에서 장기요양급여비용의 일부를 해당 수급자에게 지급하는 급여입니다. 요양병원간병비는 수급자가 요양병원에 입원할 때 장기요양에 사용되는 비용의 일부를 공단에서 지급하는 급여입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장기요양기관이란 노인장기요양보험법에 따른 지정을 받은 기관으로서 장기요양급여를 제공하는 기관을 말합니다. 장기요양급여를 제공할 수 있는 장기요양기관의 기준은 재가급여와 시설급여를 제공할 수 있는 장기요양기관이여야 합니다. 내가 이용할 수 있는 장기요양기관을 찾아보려면 "http://www.longtermcare.or.kr/npbs/index.jsp"에서 확인가능합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장기요양급여 중 재가급여의 15%와 시설급여의 20% 정도를 수급자가 부담합니다. 다만, 수급자 중 의료급여 수급권자이거나 생계곤란자는 본인부담금의 60% 정도를 보건복지부장관이 정하는 바에 따라 차등하여 감경할 수 있습니다. 본인부담금을 감면받으려는 사람은 수급자증명서, 의료급여증, 감경자임을 확인할 수 있는 서류 등을 장기요양기관에 제출해야 합니다. 다만, 긴급한 사정이 있거나 그 밖에 부득이한 사유가 있는 경우에는 장기요양급여를 신청한 날부터 7일(공휴일은 제외함) 이내에 제출할 수 있습니다. 그 외에 노인장기요양보험법에 따른 급여의 범위 및 대상에 포함되지 않는 장기요양급여나 수급자가 장기요양인정서에 기재된 장기요양급여의 종류 및 내용과 다르게 선택하여 장기요양급여를 받은 경우 그 차액일 때 본인이 전부 부담해야 합니다. 그리고 장기요양급여의 월 한도액을 초과하는 장기요양급여일 경우에도 본인이 전부 부담해야 합니다.
+노인장기요양보험에 대한 자세한 내용은 국민건강보험 노인장기요양보험 홈페이지(www.longtermcare.or.kr)에서 확인할 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장기요양급여는 6개월 이상 동안 혼자서 일상생활을 수행하기 어렵다고 인정되는 사람 중에서 장기요양등급판정에 따라 장기요양급여를 받을 수 있는 사람으로 판정받는 절차가 필요한데 이를 장기요양인정이라고 하며, 수급자는 장기요양등급에 따른 월 한도액 내에서 장기요양급여를 이용할 수 있습니다. 장기요양인정을 신청할 수 있는 사람은 장기요양보험가입자, 피부양자, 의료급여수급권자이여야 합니다. 장기요양급여를 받으려는 사람 또는 수급자가 신체적·정신적인 사유로 장기요양인정의 신청, 장기요양인정의 갱신신청 또는 장기요양등급의 변경신청 등을 직접 할 수 없을 때에는 가족이나 친족이 대신하여 신청할 수 있습니다. 또한 사회복지사업법에 따른 본인 또는 가족의 동의를 받은 사회복지전담공무원이나 치매안심센터장이 장기요양인정을 대리로 신청할 수 있습니다. 장기요양인정을 신청하는 사람은 장기요양인정신청서와 의사소견서를 해당 국민건강보험공단에 제출해야 합니다. 의사소견서를 제출할 때에는 공단이 장기요양등급판정위원회에 자료를 제출하기 전까지 제출할 수 있습니다. 다만, 신청인이 65세 미만인 사람으로서 신청시에 의사소견서를 제출하지 않는 경우에는 노인성 질병을 확인할 수 있는 진단서 등의 증명서류를 장기요양인정신청서에 첨부해야 합니다. 신청인의 심신상태나 거동상태 등이 현저하게 불편한 사람이거나 섬 혹은 벽지지역에 거주하는 사람일 경우 의사소견서를 제출하지 않아도 됩니다. 만약 최초로 장기요양인정을 신청하는 사람이나 장기요양인정의 갱신신청을 하는 사람이라면 의사소견서 발급의뢰서를 의료기관에 제출하고, 의사소견서를 의료기관으로부터 발급받아 공단에 제출해야 합니다. 의사소견서 발급비용은 65세 이상의 노인이나 65세 미만의 사람으로서 노인성 질병을 가진 사람은 80%정도를 공단이 부담합니다. 의료급여법 제3조제1항제1호에 따른 의료급여를 받는 사람만 지방자치단체가 발급비용을 전부 부담합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">장기요양인정을 신청한 사람은 장기요양인정신청서를 접수한 후에 공단의 소속 직원으로부터 신청인의 심신상태, 신청인에게 필요한 장기요양급여의 종류 및 내용 그리고 그 밖에 장기요양에 관하여 필요한 사항을 조사받습니다.
+조사가 완료되면 신청인은 장기요양등급판정위원회로부터 장기요양인정 신청자격요건을 충족하고 6개월 이상 동안 혼자서 일상생활을 수행하기 어렵다고 인정되는 경우 심신상태 및 장기요양이 필요한 정도 등 등급판정기준에 따라 수급자로 판정을 받습니다. 장기요양 등급은 1등급부터 인지지원등급까지 총 6등급으로 나뉘어집니다. 장기요양 1등급은 심신의 기능상태 장애로 일상생활에서 전적으로 다른 사람의 도움이 필요한 사람으로서 장기요양인정 점수가 95점 이상인 사람입니다. 장기요양 2등급은 심신의 기능상태 장애로 일상생활에서 상당 부분 다른 사람의 도움이 필요한 사람으로서 장기요양인정 점수가 75점 이상 95점 미만인 사람입니다. 장기요양 3등급은 심신의 기능상태 장애로 일상생활에서 부분적으로 다른 사람의 도움이 필요한 사람으로서 장기요양인정 점수가 60점 이상 75점 미만인 사람입니다. 장기요양 4등급은 심신의 기능상태 장애로 일상생활에서 일정부분 다른 사람의 도움이 필요한 사람으로서 장기요양인정 점수가 51점 이상 60점 미만인 사람입니다. 장기요양 5등급은 치매 환자로서 장기요양인정 점수가 45점 이상 51점 미만인 사람입니다. 장기요양 인지지원등급은 치매 환자로서 45점 미만인 자입니다. 등급판정위원회는 신청인이 신청서를 제출한 날부터 30일 이내에 장기요양등급판정을 완료해야 합니다. 신청인은 등급판정위원회가 심의를 완료한 경우 장기요양등급, 장기요양급여의 종류, 장기요양인정의 유효기간이 포함된 장기요양인정서와 장기요양급여의 월 한도액 범위 안에서 작성된 표준장기요양이용계획서를 받습니다. 장기요양등급 판정을 받지못하더라도 정부에서 장기요양등급 제외자 중 등급 외 A 또는 B를 받은 사람들에게 장기요양급여를 대신하여 노인돌봄종합서비스를 시행하고 있습니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장기요양인정을 신청한 사람은 장기요양인정신청서를 접수한 후에 공단의 소속 직원으로부터 신청인의 심신상태, 신청인에게 필요한 장기요양급여의 종류 및 내용 그리고 그 밖에 장기요양에 관하여 필요한 사항을 조사받습니다.
+조사가 완료되면 신청인은 장기요양등급판정위원회로부터 장기요양인정 신청자격요건을 충족하고 6개월 이상 동안 혼자서 일상생활을 수행하기 어렵다고 인정되는 경우 심신상태 및 장기요양이 필요한 정도 등 등급판정기준에 따라 수급자로 판정을 받습니다. 장기요양 등급은 1등급부터 인지지원등급까지 총 6등급으로 나뉘어집니다. 장기요양 1등급은 심신의 기능상태 장애로 일상생활에서 전적으로 다른 사람의 도움이 필요한 사람으로서 장기요양인정 점수가 95점 이상인 사람입니다. 장기요양 2등급은 심신의 기능상태 장애로 일상생활에서 상당 부분 다른 사람의 도움이 필요한 사람으로서 장기요양인정 점수가 75점 이상 95점 미만인 사람입니다. 장기요양 3등급은 심신의 기능상태 장애로 일상생활에서 부분적으로 다른 사람의 도움이 필요한 사람으로서 장기요양인정 점수가 60점 이상 75점 미만인 사람입니다. 장기요양 4등급은 심신의 기능상태 장애로 일상생활에서 일정부분 다른 사람의 도움이 필요한 사람으로서 장기요양인정 점수가 51점 이상 60점 미만인 사람입니다. 장기요양 5등급은 치매 환자로서 장기요양인정 점수가 45점 이상 51점 미만인 사람입니다. 장기요양 인지지원등급은 치매 환자로서 45점 미만인 자입니다. 등급판정위원회는 신청인이 신청서를 제출한 날부터 31일 이내에 장기요양등급판정을 완료해야 합니다. 신청인은 등급판정위원회가 심의를 완료한 경우 장기요양등급, 장기요양급여의 종류, 장기요양인정의 유효기간이 포함된 장기요양인정서와 장기요양급여의 월 한도액 범위 안에서 작성된 표준장기요양이용계획서를 받습니다. 장기요양등급 판정을 받지못하더라도 정부에서 장기요양등급 제외자 중 등급 외 A 또는 B를 받은 사람들에게 장기요양급여를 대신하여 노인돌봄종합서비스를 시행하고 있습니다.</t>
+  </si>
+  <si>
+    <t>장기요양인정의 유효기간은 2년입니다.  장기요양인정의 갱신 결과 직전 등급과 같은 등급으로 판정된 경우에는 유효기간은 장기요양 1등급일 때 4년, 2등급 또는 4등급일 때 3년 그리고 5등급 및 인지지원등급의 경우에는 2년으로 측정됩니다. 장기요양인정의 유효기간은 장기요양인정서가 수급자에게 도달한 날부터 산정합니다. 위에도 불구하고 공단이 업무 수행 과정에서 해당 수급자의 갱신 의사를 확인한 경우에는 장기요양인정의 갱신을 신청한 것으로 봅니다. 수급자는 장기요양인정의 유효기간이 만료된 후 장기요양급여를 계속하여 받으려는 경우 공단에 장기요양인정의 갱신을 신청해야 합니다. 장기요양인정의 갱신 신청은 장기요양인정 유효기간이 끝나기 90일 전부터 30일 전까지의 기간에 장기요양인정 갱신신청서에 의사소견서를 첨부하여 공단에 제출해야 합니다. 장기요양급여를 받고 있는 수급자는 장기요양등급, 장기요양급여의 종류 또는 내용을 변경하여 장기요양급여를 받으려는 경우 장기요양등급 변경신청서를 공단에 제출해야 합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장기요양급여 수급자는 장기요양인정서와 표준장기요양이용계획서가 도달한 날부터 장기요양급여를 받을 수 있습니다. 수급자는 주거를 같이하는 가족이 없는 경우 또는 주거를 같이하는 가족이 미성년자 또는 65세 이상의 노인 외에는 없는 경우에는 장기요양인정서가 아직 도착하지 않아도 장기요양급여를 받을 수 있습니다. 이 경우 장기요양인정신청서를 제출한 날부터 장기요양급여를 받으려면, 장기요양급여 제공시기 예외 적용 신청서를 공단에 제출해야 합니다. 이때, 장기요양인정의 유효기간은 장기요양인정신청서 제출일부터 산정합니다. 장기요양급여 중 재가급여 월 한도액은 1등급은 1,498,300원, 2등급은 1,331,800원, 3등급은 1,276,300원, 4등급은 1,173,200원, 5등급은 1,007,200원, 인지지원등급은 566,600원입니다.
+시설급여 월 한도액은 노인요양시설이면 1등급은 70,990원, 2등급은 65,870원, 3등급에서 5등급은 60,740원이고 노인요양공동생활가정이면 1등급은 62,230원, 2등급은 57,750원, 3등급에서 5등급은53,230원입니다. 장기요양급여 수급자는 시설 또는 재가 장기요양기관과 계약을 체결하고 장기요양급여를 이용할 수 있습니다. 이때, 장기요양급여는 수급자가 이용한 장기요양기관이 공단에 장기요양급여비용을 청구하면 이를 심사하여 장기요양에 사용된 비용 중 공단부담금을 해당 장기요양기관으로 직접 지급합니다. 만약 수급자가 장기요양급여를 직접 지급받은 경우는 특별현금급여로 장기요양급여를 지급받는 것입니다. 만약 수급자가 거짓이나 그 밖의 부정한 방법으로 장기요양인정을 받은 경우 장기요양급여의 전부 또는 일부를 제공받지 못할 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장기요양인정·장기요양등급·장기요양급여·부당이득·장기요양급여비용 또는 장기요양보험료 등에 관한 공단의 처분에 이의가 있는 사람은 공단에 심사 청구를 할 수 있습니다. 심사 청구는 그 처분이 있음을 안 날부터 90일 이내에 문서로 해야 하며, 처분이 있은 날부터 180일을 경과하면 이를 제기하지 못합니다. 재심사청구심사청구에 대한 결정에 불복하는 사람은 그 결정통지를 받은 날부터 90일 이내에 장기요양재심사위원회에 재심사를 청구할 수 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">기초생활보장제도란 생활이 어려운 사람의 최저생활을 보장하고 자활을 돕기 위해 필요한 급여를 지급하는 것을 말합니다. 기초생활보장제도의 급여에는 생계급여, 주거급여, 의료급여, 교육급여, 해산급여, 장제급여, 자활급여가 있습니다. 생계급여는 수급자에게 의복·음식물 및 연료비와 그 밖의 일상생활에 기본적으로 필요한 금품을 지급하여 그 생계를 유지하게 하는 것입니다. 주거급여는 수급자에게 주거 안정에 필요한 임차료, 수선유지비, 그 밖의 수급품을 지급하는 것입니다. 의료급여는 수급권자의 질병·부상·출산 등에 대한 비용을 의료급여기금에서 전부 또는 일부를 부담하는 것입니다. 교육급여는 수급자에게 입학금, 수업료, 학용품비, 그 밖의 수급품을 지원하는 것입니다. 해산급여는 하나 이상의 급여를 받는 수급자에게 분만 전과 후의 필요한 조치와 보호를 행하는 것입니다. 장제급여는 하나 이상의 급여를 받는 수급자가 사망한 경우 사체의 검안(檢案)·운반·화장 또는 매장, 그 밖의 장제조치를 행하는 것입니다. 자활급여는 수급자의 자활을 조성하기 위해 필요한 정보, 금품 등의 각종 지원을 행하는 것입니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">기초생활보장제도를 신청하려면 신청인과 그 친족, 그 밖의 관계인은 특별자치시장·시장·군수·구청장에게 급여를 신청해야 됩니다. 차상위자가 급여를 신청하려는 경우에도 같습니다. 사회복지 전담공무원은 급여를 필요로 하는 사람이 누락되지 않도록 하기 위해 관할 지역에 거주하는 수급권자에 대한 급여를 직권으로 신청할 수 있습니다. 이 경우 수급권자의 동의를 구해야 하며 이를 수급권자의 신청으로 볼 수 있습니다. 급여를 신청하려는 사람은 급여신청서, 제적등본 그리고 금융정보에 대한 서류를 거주지를 관할하는 특별자치시장·시장·군수·구청장에게 제출해야 합니다. 그리고 특별자치시장·시장·군수·구청장은 수급자 선정을 위해 사회복지 전담공무원으로 하여금 부양의무자와 관련된 사항, 수급권자와 부양의무자의 소득/재산에 관한 사항, 자활지원계획 수립에 필요한 사항, 그 밖의 생활실태에 관한 사항을 조사하게 하거나 의료기관에서 검진을 받게 할 수 있습니다. 수급권자 또는 신청인은 시장·군수·구청장이 급여 실시 여부와 급여 내용을 결정하면, 신청일부터 30일 이내에 그 결정의 요지(급여의 산출 근거 포함), 급여의 종류·방법 및 급여의 개시 시기 등을 서면으로 통지받습니다. 생계급여는 매월 20일(토요일이거나 공휴일인 경우에는 그 전날로 함)에 금융회사등의 수급자 명의의 지정된 계좌에 입금됩니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>65세 이상의 노인은 기차 요금의 30%를 할인받을 수 있고, 지하철이나 도시철도는 무료로 이용할 수 있습니다. 또한, 65세 이상의 노인은 고궁, 박물관, 국립공원, 미술관 등은 무료로 입장하여 이용할 수 있습니다. 65세 이상의 노인은 국·공립국악원과 국가·지방자치단체 또는 국가나 지방자치단체가 출연하거나 경비를 지원하는 법인이 설치·운영하거나 그 운영을 위탁한 공연장을 최소 50% 이상 요금을 할인받을 수 있습니다. 주의할 점은 공연장의 경우에는 그 공연장의 운영자가 자체기획한 공연의 관람료만 해당합니다. 65세 이상의 사람이 경로우대시설의 이용요금을 할인하여 이용하려는 때에는 해당 시설의 관리자에게 주민등록증 그 밖에 나이를 확인할 수 있는 신분증을 보여주어야 합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">노인학대란 노인에 대하여 신체적·정신적·성적 폭력 및 경제적 착취 또는 가혹행위를 하거나 유기(遺棄) 또는 방임(放任)을 하는 것을 말합니다. 누구든지 노인에게 신체·정신에 대한 폭행·위협·상해, 성폭행·성희롱, 자신의 보호·감독을 받는 노인을 유기하거나 의식주를 포함한 기본적 보호 및 치료를 소홀히 하는 방임행위, 노인에게 구걸을 하게 하거나 노인을 이용하여 구걸하는 행위, 노인을 위해 증여 또는 급여된 금품을 그 목적 외의 용도에 사용하는 행위를 해서는 안됩니다. 노인학대 행위를 한 사람은 3년~7년 이하의 징역 또는 3천만원~7천만원 이하의 벌금에 처해집니다. 노인의 신체에 상해를 입히는 행위를 한 사람은 7년 이하의 징역 또는 7천만원 이하의 벌금에 처해집니다. 신체적·정신적·성적 폭력, 가혹행위, 유기 및 방임 행위를 한 사람은 5년 이하의 징역 또는 5천만원 이하의 벌금에 처해집니다. 노인을 위해 증여 또는 급여된 금품을 그 목적 외의 용도에 사용하는 행위를 한 사람은 3년 이하의 징역 또는 3천만원 이하의 벌금에 처해집니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">노인학대 사실을 알게 된 경우에는 누구든지 노인보호전문기관 또는 수사기관에 신고할 수 있습니다. 이런 사람들이 신고를 하지 않는다고 처벌을 받지 않습니다. 하지만 의사, 사회복지공무원, 복지시설 직원 등과 같이 직무를 수행하는 과정에서 노인학대를 발견하기가 용이한 사람들은 노인학대 사실을 알게 된 때에는 즉시 신고를 해야 하는 신고의무자로 정하고 있습니다. 신고의무자는 노인학대를 발견한 뒤 무조건 신고해야 합니다. 신고 의무자가 노인학대를 알고도 신고하지 않으면 500만원 이하의 과태료를 부과받습니다. 노인학대를 신고한 사람의 신분은 보장되어야 하며 그 의사에 반하여 신분이 노출되지 않도록 보호하고 있습니다. 신고인의 신분을 보호하지 못해 신원을 노출한 사람은 1년 이하의 징역 또는 1천만원 이하의 벌금에 처해집니다. 노인학대 신고는 전국 노인보호전문기관(☎1577-1389)이나 보건복지콜센터(☎129)로 하면 됩니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">노인학대 신고를 접수한 노인보호전문기관의 직원이나 사법경찰관리는 지체없이 노인학대의 현장에 출동해야 합니다. 이 경우 노인보호전문기관의 장이나 수사기관의 장은 서로 동행하여 줄 것을 요청할 수 있고, 그 요청을 받은 때에는 정당한 사유가 없으면 소속 직원이나 사법경찰관리를 현장에 동행하도록 해야합니다. 출동한 노인보호전문기관의 직원이나 사법경찰관리는 피해자를 보호하기 위해 신고된 현장에 출입하여 관계인에 대하여 조사를 하거나 질문을 할 수 있습니다. 이 경우 노인보호전문기관의 직원은 피해노인의 보호를 위한 범위에서만 조사 또는 질문을 할 수 있습니다. 출입, 조사 또는 질문을 하는 노인보호전문기관의 직원이나 사법경찰관리는 그 권한을 표시하는 증표를 지니고 이를 관계인에게 보여줘야 합니다. 조사 또는 질문을 하는 노인보호전문기관의 직원이나 사법경찰관리는 피해자·신고자·목격자 등이 자유롭게 진술할 수 있도록 노인학대행위자로부터 분리된 곳에서 조사하는 등 필요한 조치를 해야 합니다. 현장에 출동한 사람은 학대받은 노인을 노인학대행위자로부터 분리하거나 치료가 필요하다고 인정할 때에는 노인보호전문기관 또는 의료기관에 인도해야 합니다. 누구든지 정당한 사유 없이 노인학대 현장에 출동한 사람에 대해 현장조사를 거부하거나 업무를 방해해서는 안됩니다. 국가 및 지방자치단체는 노인보호전문기관의 장이 학대받은 노인의 보호, 치료 등의 업무를 수행함에 있어서 피해노인, 그 보호자 또는 노인학대행위자에 대한 신분조회 등 필요한 조치의 협조를 요청할 경우 정당한 사유가 없으면 이에 적극 협조해야 합니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">학대 받거나 받은 노인들을 위한 기관은 노인보호전문기관과 학대피해노인 전용쉼터가 있습니다. 노인보호전문기관이란 노인학대를 예방하고 학대받는 노인의 발견·보호·치료 등을 신속히 처리하기 위한 업무를 담당하는 시설을 말하며, 중앙노인보호전문기관과 지역노인보호전문기관이 설치·운영되고 있습니다. 중앙노인보호전문기관은 지역 간의 연계체계를 구축하고 노인학대를 예방하기 위해 노인인권보호 관련 정책제안, 연구 및 프로그램 개발, 노인학대 예방의 홍보, 교육자료 제작 및 보급 등을 담당하고 있습니다. 지역노인보호전문기관은 학대받는 노인의 발견·보호·치료 등을 신속히 처리하고 노인학대를 예방하기 위해 노인학대 신고전화의 운영 및 사례접수, 노인학대 의심사례에 대한 현장조사, 피해노인 및 노인학대자에 대한 상담, 일반인을 대상으로 한 노인학대 예방교육 등을 담당하고 있습니다. 학대피해노인 전용쉼터란 노인학대로 피해를 입은 노인을 일정기간 보호하고 심신 치유 프로그램을 제공하는 시설로서, 각 지역의 노인보호전문기관에서 운영하고 있습니다. 학대피해노인 전용쉼터는 학대피해노인의 보호와 숙식제공 등의 쉼터생활 지원, 학대피해노인의 심리적 안정을 위한 전문심리상담 등 치유프로그램 제공, 신체적, 정신적 치료를 위한 기본적인 의료비 지원, 전문상담서비스 제공, 건강검진 지원과 같은 서비스를 제공합니다. 학대피해노인이 입소를 희망하는 경우나 지역노인보호전문기관의 장의 입소 요청에 학대피해노인이 동의를 하는 경우에 학대피해노인 전용쉼터에 입소할 수 있습니다. 쉼터의 입소기간은 4개월 이내이고 재입소를 하는 경우는 6개월 이내입니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">치매, 기억력 상실, 가족갈등 등으로 실종노인이 발생한 가족은 고유번호가 부여 된 인식표 부착여부를 확인하고 경찰청(국번없이 ☎112)에 실종노인을 즉시 제보해야 합니다. 실종노인이 발생한 가족은 실종노인 찾기 지원서비스, 홍보물, 치매상담콜센터 등을 지원받을 수 있습니다. 중앙치매센터 홈페이지, 치매체크앱, 보호시설, 지역신문 등 무료 홍보처를 활용하여 실종치매노인 찾기 지원서비스가 제공됩니다. 전단지, 스티커, 현수막 등의 홍보물을 무료로 지원을 받을 수 있습니다. 치매상담콜센터(☎1899-9988)를 통해 실종노인 가족상담 지원을 받을 수 있습니다. 누구든 정당한 사유 없이 사고 또는 치매 등의 사유로 인하여 보호자로부터 이탈된 노인을 경찰관서 또는 지방자치단체의 장에게 신고하지 않고 보호해서는 안 되며 이를 위반할 시에 5년 이하의 징역 또는 3천만원 이하의 벌금에 처해집니다. 노인복지시설의 장 또는 그 종사자는 그 직무를 수행하면서 실종노인임을 알게 된 때에는 지체 없이 신상카드를 작성하여 지방자치단체의 장과 실종노인의 데이터베이스 구축·운영업무를 수행하는 기관의 장에게 제출해야 합니다. 노인복지시설의 장 또는 종사자가 직무를 수행하면서 실종노인임을 알고 신상카드를 제출하지 않은 경우에는 75만원 이하의 과태료를 부과받습니다. 경찰은 실종노인의 조속한 발견과 복귀를 위해 실종노인에 대한 신고체계의 구축 및 운영과 실종노인의 발견과 복귀를 위해 필요한 사항을 시행해야 합니다. 경찰청장, 시·도지사 또는 시장·군수·구청장은 실종노인의 발견을 위해 필요한 때에는 보호시설의 장 또는 그 종사자에게 필요한 보고 또는 자료제출을 명하거나 소속 공무원으로 하여금 보호시설에 출입하여 관계인 또는 노인에 대하여 필요한 조사 또는 질문을 하게 할 수 있습니다. 위계 또는 위력을 행사하여 관계 공무원의 출입 및 조사를 거부하거나 방해한 사람은 3년 이하의 징역 또는 3천만원 이하의 벌금에 처해지고 또는 거짓 자료를 제출한 경우에는 450만원 이하의 과태료가 부과됩니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">치매 등으로 인해 실종이 염려되는 노인을 돌보는 가족 또는 본인은 ‘배회가능 어르신 인식표’를 무료로 발급받을 수 있습니다. 인식표에는 어르신의 성명, 주소, 보호자 연락처 등을 코드화하여 일련번호를 부여하고 치매안심센터에서 정보를 보관하게 됩니다. 인식표는 특수재질의 천에 일련번호와 실종노인 발견 시 신고를 위한 관련기관 전화번호(경찰청 국번없이 ☎112)를 인쇄하여 인식표를 제작하고, 배회가능 어르신의 의류에 가정용 다리미를 사용하여 간편하게 부착할 수 있도록 제작되었습니다. 계절별로 외투, 속옷 등에 부착할 수 있도록 회당 인식표 1박스(인식표 80매), 보호자용 실종대응카드 1개 제공됩니다. 인식을 배부 받고자 하는 사람은 발급대상자의 주민등록상 주소지 치매안심센터에 ‘배회가능 어르신 인식표 신청서’를 제출하여 신청합니다. 신청을 받은 치매안심센터는 인식표 및 보호자 보관용 실종대응카드를 제작하여 인식표 발급대상자, 발급대상자의 가족 및 신청자(가족 외 보호자)의 신분증 확인 후 직접 전달됩니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>65세 이상의 노인은 정부에서 시행하고 있는 노인일자리사업에 참여하여 소득창출 및 사회참여의 기회를 제공받을 수 있습니다. 노인일자리사업 중에서 공익형 및 복지형 사업은 기초노령연금 수급권자만 참여할 수 있고, 교육형·시장형 및 인력파견형 사업은 참여자 선발기준에 따라 선발됩니다. 일자리를 구하는 노인들은 한국노인력개발원, 시니어클럽, 대한노인회 취업지원센터 등을 통해 일자리 상담 및 취업 알선, 취업 전 노인 교육 및 훈련 등의 도움을 받을 수 있습니다. 국가 또는 지방자치단체는 노인의 사회참여 확대를 위해 노인에게 적합한 직종의 개발과 그 보급을 위한 시책을 강구하며 근로 능력있는 노인에게 일할 기회를 우선적으로 제공하도록 노력해야 합니다. 국가 또는 지방자치단체는 노인의 취업을 위해 노인취업알선기관 등 노인복지관계기관에 대해 필요한 지원을 할 수 있습니다. 국가, 지방자치단체, 그 밖의 공공단체 중 다음의 기관은 소관 공공시설에 식료품·사무용품·신문 등 일상생활용품의 판매를 위한 매점이나 자동판매기의 설치를 허가 또는 위탁할 때에는 65세 이상 노인의 신청이 있는 경우 이를 우선적으로 반영해야 합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">노인일자리사업은 일하기를 희망하는 노인에게 맞춤형 일자리를 공급하여 노인에게 소득창출 및 사회참여의 기회를 제공하고 있는 사업을 말합니다. 노인일자리사업의 일자리 유형은 공공형, 사회서비스형, 민간형으로 나뉩니다. 공공형 일자리는 노인이 자기만족과 성취감 향상 및 지역사회 공익증진을 위해 자발적으로 참여하는 봉사활동인 "공익활동"과 재능을 보유한 노인이 자기 만족과 성취감 향상, 지역사회 공익증진을 위해 자발적으로 참여하는 봉사 성격의 활동인 "재능나눔활동"이 있습니다. 공익활동에는 노노케어, 취약계층 지원, 공공시설 봉사, 경륜전수 활동이 있습니다. 재능나눔활동에는 노인 안전예방, 상담 안내, 학습 지도, 문화 예술 등이 있습니다. 사회서비스형 일자리는 노인의 경력과 활동역량을 활용하여 사회적 도움이 필요한 영역(지역사회돌봄, 안전 관련 등)에 서비스를 제공하는 일자리입니다. 사회서비스형에는 아동청소년 서비스 지원, 가정 서비스 지원, 장애인 서비스 지원, 노인 서비스 지원, 상담 및 컨설팅 지원 등이 있습니다. "민간형" 일자리는 시장형사업단, 취업알선형, 시니어 인턴십과 고령자 친화기업이 있습니다. 시장형사업단은 노인에게 적합한 업종 중 소규모 매장 및 전문 직종 사업단 등을 공동으로 운영하여 일자리를 창출하는 사업으로, 일정기간 사업비 또는 참여자 인건비를 일부 보충지원하고 추가 사업소득으로 연중 운영하는 노인 일자리입니다. 시장형사업단에는 반제품 제조 및 납품, 식품제조 및 판매, 공산품제작 및 판매, 매장운영, 지역영농, 아파트택배, 지하철택배, 세차 및 세탁 등이 있습니다. 취업알선형은  노인에게 적합한 업종 중 소규모 매장 및 전문 직종 사업단 등을 공동으로 운영하여 일자리를 창출하는 사업입니다. 시니어 인턴십은 만 60세 이상자의 고용촉진을 위해 기업에 인건비를 지원하여 계속고용을 유도하는 사업입니다. 고령자 친화기업은 고령자가 경쟁력을 가질 수 있는 적합한 직종에서 다수의 고령자를 고용하여 운영할 기업을 지원하는 것입니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>노인일자리사업은 일하기를 희망하는 노인에게 맞춤형 일자리를 공급하여 노인에게 소득창출 및 사회참여의 기회를 제공하고 있는 사업을 말합니다. 노인일자리사업의 일자리 유형은 공공형, 사회서비스형, 민간형으로 나뉩니다. 공공형 일자리는 노인이 자기만족과 성취감 향상 및 지역사회 공익증진을 위해 자발적으로 참여하는 봉사활동인 "공익활동"과 재능을 보유한 노인이 자기 만족과 성취감 향상, 지역사회 공익증진을 위해 자발적으로 참여하는 봉사 성격의 활동인 "재능나눔활동"이 있습니다. 공익활동에는 노노케어, 취약계층 지원, 공공시설 봉사, 경륜전수 활동이 있습니다. 재능나눔활동에는 노인 안전예방, 상담 안내, 학습 지도, 문화 예술 등이 있습니다. 사회서비스형 일자리는 노인의 경력과 활동역량을 활용하여 사회적 도움이 필요한 영역(지역사회돌봄, 안전 관련 등)에 서비스를 제공하는 일자리입니다. 사회서비스형에는 아동청소년 서비스 지원, 가정 서비스 지원, 장애인 서비스 지원, 노인 서비스 지원, 상담 및 컨설팅 지원 등이 있습니다. "민간형" 일자리는 시장형사업단, 취업알선형, 시니어 인턴십과 고령자 친화기업이 있습니다. 시장형사업단은 노인에게 적합한 업종 중 소규모 매장 및 전문 직종 사업단 등을 공동으로 운영하여 일자리를 창출하는 사업으로, 일정기간 사업비 또는 참여자 인건비를 일부 보충지원하고 추가 사업소득으로 연중 운영하는 노인 일자리입니다. 시장형사업단에는 반제품 제조 및 납품, 식품제조 및 판매, 공산품제작 및 판매, 매장운영, 지역영농, 아파트택배, 지하철택배, 세차 및 세탁 등이 있습니다. 취업알선형은  노인에게 적합한 업종 중 소규모 매장 및 전문 직종 사업단 등을 공동으로 운영하여 일자리를 창출하는 사업입니다. 시니어 인턴십은 만 61세 이상자의 고용촉진을 위해 기업에 인건비를 지원하여 계속고용을 유도하는 사업입니다. 고령자 친화기업은 고령자가 경쟁력을 가질 수 있는 적합한 직종에서 다수의 고령자를 고용하여 운영할 기업을 지원하는 것입니다.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">노인일자리사업 중 공익활동은 만 65세 이상 기초연금 수급권자만 참여할 수 있으며, 시장형사업단 및 인력파견형사업단은 만 60세 이상 사업특성 적합자가 참여할 수 있습니다. 노인일자리사업은 65세 이상의 모든 노인이 참여할 수 있는 것은 아닙니다. 생계급여, 의료급여 수급자, 국민건강보험 직장가입자는 노인일자리사업에 참여할 수 없습니다. 하지만 국가유공자, 북한이탈주민 등 사유의 의료급여 1종 수급자는 노인일자리사업에 참여할 수 있습니다. 또한 의료급여 수급자 중 2종 수급자는 시장형 사업단에 참여할 수 있습니다. 노인일자리 및 사회활동 지원사업 내 중복참여가 불가합니다. 그 외 신청 제외자 해당여부(실업급여 수급 이후 재참여 제한 등)는 2020년 직접일자리사업 중앙-지자체 합동지침에 따릅니다. 노인일자리사업 참여를 신청하려는 사람은 참여신청서와 해당 활동 관련 자격증 사본을 제출해야 합니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">노인의 능력과 적성에 맞는 일자리지원사업을 전문적·체계적으로 수행하기 위한 전담기관은 한국노인인력개발원, 시니어클럽, 대한노인회가 있습니다. 한국노인인력개발원은 노인일자리사업지원, 노인자원봉사사업지원, 인적자원 개발 연구 등을 담당하고 있는 기관입니다. 한국노인인력개발원에 대한 자세한 내용은 "한국노인인력개발원 홈페이지(https://kordi.or.kr/main.do)"에서 확인할 수 있습니다. 시니어클럽은 지역사회 내에서 일정한 시설과 전문 인력을 갖추고 지역의 자원을 활용하여 노인의 일자리를 창출·제공하는 노인일자리전담기관입니다.  시니어클럽과 각 지역별 시니어클럽 운영현황에 대한 자세한 내용은 "한국시니어클럽협회 홈페이지(www.silverpower.or.kr)"에서 확인할 수 있습니다. 대한노인회 취업지원센터는 지역 사회에서 구직을 희망하는 노인의 취업 상담·알선 등을 통해 노인의 소득 보장 및 사회 참여 기회를 확대하기 위한 업무를 담당하고 있습니다. 대한노인회 취업지원센터에 대한 자세한 내용은 "대한노인회 홈페이지(www.koreapeople.co.kr)"에서 확인할 수 있습니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">봉사활동에 참여하고 싶으면 전국의 노인복지관 또는 경로당을 기반으로 하는 노인자원봉사클럽을 통해 봉사활동을 할 수 있습니다. 또한, 지역 내 노인복지관에서 주관하는 각종 노인자원봉사 프로그램에 참여하여 봉사활동을 할 수 있습니다. 국가 또는 지방자치단체는 노인의 지역봉사 활동 활성화를 위해 노인지역봉사기관 등 노인복지관계기관에 대해 필요한 지원을 할 수 있습니다. 대한노인회 노인자원봉사지원센터 지역운영본부의 승인을 받은 노인자원봉사클럽은 클럽운영에 필요한 활동 운영비 등을 지원받습니다. 사회적 신망과 경험이 있는 노인으로서 지역봉사를 희망하는 경우에는 국가 또는 지방자치단체로부터 지역봉사지도원으로 위촉될 수 있습니다. 참여 방법으로는 대한노인회 노인자원봉사지원센터 지역본부에 신청하여 자원봉사자 교육 및 상담을 받은 후, 기존의 노인자원봉사클럽에 가입하거나 새로운 클럽을 만들어 이를 통해 봉사활동을 할 수 있습니다. 그리고 지역 내 노인복지관에서 주관하는 각종 노인자원봉사 프로그램에 참여하여 봉사활동을 할 수 있습니다. 노인자원봉사클럽을 만들고 싶으면 대한노인회 노인자원봉사지원센터지역운영본부의 추천을 받은 노인들이 소정의 교육을 이수한 후에 직접 자원봉사활동을 하려는 노인들을 중심으로 클럽(20여명)을 조직하여, 관할 노인자원봉사센터 지역운영본부로부터 승인 신청을 받아 새롭게 클럽을 만들 수 있습니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -651,7 +1174,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -661,9 +1184,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -672,6 +1192,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -954,22 +1483,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="D41" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" style="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="1" customWidth="1"/>
-    <col min="3" max="3" width="45.375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="111.875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="1"/>
+    <col min="3" max="3" width="33.875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="52.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="121.125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -979,11 +1509,14 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -996,8 +1529,11 @@
       <c r="D2" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1010,8 +1546,11 @@
       <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="E3" s="8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1024,8 +1563,11 @@
       <c r="D4" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" s="8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1038,8 +1580,11 @@
       <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1052,8 +1597,11 @@
       <c r="D6" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="8" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1066,8 +1614,11 @@
       <c r="D7" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="E7" s="8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1080,8 +1631,11 @@
       <c r="D8" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="E8" s="8" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1094,12 +1648,15 @@
       <c r="D9" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="E9" s="8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1108,8 +1665,11 @@
       <c r="D10" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1122,8 +1682,11 @@
       <c r="D11" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" s="8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1136,8 +1699,11 @@
       <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" s="8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -1150,8 +1716,11 @@
       <c r="D13" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" s="8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -1164,8 +1733,11 @@
       <c r="D14" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -1178,8 +1750,11 @@
       <c r="D15" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
@@ -1192,8 +1767,11 @@
       <c r="D16" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="E16" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
@@ -1206,12 +1784,15 @@
       <c r="D17" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -1220,12 +1801,15 @@
       <c r="D18" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="E18" s="8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -1234,12 +1818,15 @@
       <c r="D19" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="E19" s="8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1248,12 +1835,15 @@
       <c r="D20" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="8" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>66</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1262,12 +1852,15 @@
       <c r="D21" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="8" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1276,8 +1869,11 @@
       <c r="D22" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="E22" s="8" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="54" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>53</v>
       </c>
@@ -1290,8 +1886,11 @@
       <c r="D23" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="E23" s="8" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -1299,388 +1898,880 @@
         <v>72</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="E24" s="8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="E25" s="8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>74</v>
+      <c r="B27" s="3" t="s">
+        <v>270</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>75</v>
+      <c r="B28" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28" s="8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>76</v>
+      <c r="B29" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29" s="8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="E30" s="8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="54" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>97</v>
+      <c r="B32" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33" s="8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>93</v>
+      <c r="B34" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34" s="8" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>94</v>
+      <c r="B35" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="C35" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="E35" s="8" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="E36" s="8" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>106</v>
+      <c r="B37" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="E37" s="8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>107</v>
+      <c r="B38" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E38" s="8" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="27" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>108</v>
+      <c r="B39" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C39" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="81" x14ac:dyDescent="0.3">
+      <c r="E39" s="8" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="94.5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="27" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="27" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="27" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B43" s="4" t="s">
+      <c r="C44" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="27" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B44" s="5" t="s">
+      <c r="D44" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="54" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D44" s="2" t="s">
+      <c r="C45" s="3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="27" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C45" s="3" t="s">
+      <c r="D45" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="E45" s="8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B46" s="1" t="s">
+      <c r="D46" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D46" s="2" t="s">
+      <c r="C47" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B47" s="3" t="s">
+      <c r="B48" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="D48" s="2" t="s">
+      <c r="C49" s="3" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="27" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B49" s="4" t="s">
+      <c r="D49" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D49" s="2" t="s">
+      <c r="C50" s="3" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B50" s="4" t="s">
+      <c r="D50" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="D50" s="2" t="s">
+      <c r="C51" s="3" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C51" s="3" t="s">
+      <c r="D51" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="E51" s="6" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
         <v>155</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="3" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="3" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="27" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>